<commit_message>
direction change taking 1 time = bad
direction change taking 1 time = bad
but should have fluent properties eg if no change continue path
</commit_message>
<xml_diff>
--- a/situations.xlsx
+++ b/situations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruben\Desktop\Modeleren van complexe systemen\IDP-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F2F96DF-7FC0-4C95-9E40-C345F8AD3514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA183A5-BA18-45F2-945B-AA00815EAB0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D9BF9451-56DA-46F5-845C-C84CA8ADB319}"/>
+    <workbookView xWindow="28680" yWindow="240" windowWidth="25440" windowHeight="15390" xr2:uid="{D9BF9451-56DA-46F5-845C-C84CA8ADB319}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -410,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B02BB0D7-479B-48F7-B1DD-DE5A6A7F203A}">
-  <dimension ref="A1:V9"/>
+  <dimension ref="A1:V17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,6 +646,136 @@
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
     </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
draw on request handled
Structure S5 failed
</commit_message>
<xml_diff>
--- a/situations.xlsx
+++ b/situations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruben\Desktop\Modeleren van complexe systemen\IDP-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA183A5-BA18-45F2-945B-AA00815EAB0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC5A13F-5B1F-46BA-A2B4-B79893068AF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="240" windowWidth="25440" windowHeight="15390" xr2:uid="{D9BF9451-56DA-46F5-845C-C84CA8ADB319}"/>
+    <workbookView xWindow="8235" yWindow="1005" windowWidth="18900" windowHeight="11055" xr2:uid="{D9BF9451-56DA-46F5-845C-C84CA8ADB319}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,6 +32,23 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>s3</t>
+  </si>
+  <si>
+    <t>s1b</t>
+  </si>
+  <si>
+    <t>S0</t>
+  </si>
+  <si>
+    <t>s5</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -410,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B02BB0D7-479B-48F7-B1DD-DE5A6A7F203A}">
-  <dimension ref="A1:V17"/>
+  <dimension ref="A1:V37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,40 +439,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
+      <c r="C2" s="4"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="3"/>
+      <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -473,14 +470,14 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="C3" s="4"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="H3" s="3"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -498,11 +495,11 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="C4" s="4"/>
+      <c r="E4" s="3"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -523,14 +520,14 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1"/>
-      <c r="C5" s="3"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="3"/>
+      <c r="C5" s="4"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -548,14 +545,14 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="C6" s="4"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="3"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -573,14 +570,14 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="C7" s="4"/>
+      <c r="E7" s="3"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="3"/>
+      <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -598,14 +595,14 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="C8" s="4"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+      <c r="H8" s="3"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -623,11 +620,11 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>0</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="1"/>
-      <c r="E9" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="4"/>
+      <c r="E9" s="3"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -646,41 +643,45 @@
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
     </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="4"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+    </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>4</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
-      <c r="S13" s="1"/>
-      <c r="T13" s="1"/>
-      <c r="U13" s="1"/>
-      <c r="V13" s="1"/>
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>3</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="2"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="2"/>
+      <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -700,12 +701,12 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2</v>
-      </c>
-      <c r="B15" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="B15" s="2"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -726,12 +727,12 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>1</v>
-      </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="2"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -752,10 +753,10 @@
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>0</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -776,6 +777,286 @@
       <c r="U17" s="1"/>
       <c r="V17" s="1"/>
     </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>4</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+      <c r="E31">
+        <v>3</v>
+      </c>
+      <c r="F31">
+        <v>4</v>
+      </c>
+      <c r="G31">
+        <v>5</v>
+      </c>
+      <c r="H31">
+        <v>6</v>
+      </c>
+      <c r="I31">
+        <v>7</v>
+      </c>
+      <c r="J31">
+        <v>8</v>
+      </c>
+      <c r="M31">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>5</v>
+      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>4</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>3</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="2"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>2</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="1"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>0</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added doors + inv
untested invariants
</commit_message>
<xml_diff>
--- a/situations.xlsx
+++ b/situations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruben\Desktop\Modeleren van complexe systemen\IDP-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791AB7C1-F0AE-4188-B98B-1EFE4E57322B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73B7CA70-7BE7-4653-BE3F-84BF3190934F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38070" yWindow="11295" windowWidth="18900" windowHeight="11055" xr2:uid="{D9BF9451-56DA-46F5-845C-C84CA8ADB319}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{D9BF9451-56DA-46F5-845C-C84CA8ADB319}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
   <si>
     <t>s3</t>
   </si>
@@ -60,12 +60,18 @@
   <si>
     <t>s14</t>
   </si>
+  <si>
+    <t>REQUEST</t>
+  </si>
+  <si>
+    <t>Request</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,8 +79,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -105,6 +124,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -118,7 +149,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -126,6 +157,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,8 +476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B02BB0D7-479B-48F7-B1DD-DE5A6A7F203A}">
   <dimension ref="A1:V59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -826,10 +860,10 @@
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="2"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -847,9 +881,9 @@
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="2"/>
+      <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="2"/>
+      <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -864,12 +898,16 @@
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="2"/>
+      <c r="E17" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-      <c r="J17" s="2"/>
+      <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
@@ -880,22 +918,16 @@
       <c r="A18">
         <v>3</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E18" s="2"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
-      <c r="K18" s="2"/>
+      <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
@@ -905,17 +937,25 @@
       <c r="A19">
         <v>2</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
+      <c r="B19" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="2"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
-      <c r="L19" s="2"/>
+      <c r="L19" s="1"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
@@ -926,16 +966,22 @@
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="2"/>
+      <c r="D20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
     </row>

</xml_diff>

<commit_message>
during opening and closing the el will have a direction
also remove unused predicate
</commit_message>
<xml_diff>
--- a/situations.xlsx
+++ b/situations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruben\Desktop\Modeleren van complexe systemen\IDP-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754A5988-BD20-41C7-9EE3-172E53775E74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DEB02F-79E2-4C6F-B5C0-443D50D23CB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2790" yWindow="-615" windowWidth="47760" windowHeight="14145" xr2:uid="{D9BF9451-56DA-46F5-845C-C84CA8ADB319}"/>
+    <workbookView xWindow="32355" yWindow="1290" windowWidth="47760" windowHeight="14145" xr2:uid="{D9BF9451-56DA-46F5-845C-C84CA8ADB319}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>s3</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>S20</t>
+  </si>
+  <si>
+    <t>S21</t>
   </si>
 </sst>
 </file>
@@ -500,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B02BB0D7-479B-48F7-B1DD-DE5A6A7F203A}">
-  <dimension ref="A1:BX92"/>
+  <dimension ref="A1:BX102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2:S6"/>
+      <selection activeCell="AG8" sqref="AG8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,7 +521,7 @@
   <sheetData>
     <row r="1" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B1" s="11">
         <v>0</v>
@@ -528,295 +531,295 @@
         <v>1</v>
       </c>
       <c r="D1" s="11">
-        <f t="shared" ref="D1:BO1" si="0">C1+1</f>
+        <f t="shared" ref="D1" si="0">C1+1</f>
         <v>2</v>
       </c>
       <c r="E1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E1" si="1">D1+1</f>
         <v>3</v>
       </c>
       <c r="F1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="F1" si="2">E1+1</f>
         <v>4</v>
       </c>
       <c r="G1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="G1" si="3">F1+1</f>
         <v>5</v>
       </c>
       <c r="H1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="H1" si="4">G1+1</f>
         <v>6</v>
       </c>
       <c r="I1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="I1" si="5">H1+1</f>
         <v>7</v>
       </c>
       <c r="J1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="J1" si="6">I1+1</f>
         <v>8</v>
       </c>
       <c r="K1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="K1" si="7">J1+1</f>
         <v>9</v>
       </c>
       <c r="L1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="L1" si="8">K1+1</f>
         <v>10</v>
       </c>
       <c r="M1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="M1" si="9">L1+1</f>
         <v>11</v>
       </c>
       <c r="N1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="N1" si="10">M1+1</f>
         <v>12</v>
       </c>
       <c r="O1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="O1" si="11">N1+1</f>
         <v>13</v>
       </c>
       <c r="P1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="P1" si="12">O1+1</f>
         <v>14</v>
       </c>
       <c r="Q1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="Q1" si="13">P1+1</f>
         <v>15</v>
       </c>
       <c r="R1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="R1" si="14">Q1+1</f>
         <v>16</v>
       </c>
       <c r="S1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="S1" si="15">R1+1</f>
         <v>17</v>
       </c>
       <c r="T1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="T1" si="16">S1+1</f>
         <v>18</v>
       </c>
       <c r="U1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="U1" si="17">T1+1</f>
         <v>19</v>
       </c>
       <c r="V1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="V1" si="18">U1+1</f>
         <v>20</v>
       </c>
       <c r="W1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="W1" si="19">V1+1</f>
         <v>21</v>
       </c>
       <c r="X1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="X1" si="20">W1+1</f>
         <v>22</v>
       </c>
       <c r="Y1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="Y1" si="21">X1+1</f>
         <v>23</v>
       </c>
       <c r="Z1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="Z1" si="22">Y1+1</f>
         <v>24</v>
       </c>
       <c r="AA1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AA1" si="23">Z1+1</f>
         <v>25</v>
       </c>
       <c r="AB1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AB1" si="24">AA1+1</f>
         <v>26</v>
       </c>
       <c r="AC1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AC1" si="25">AB1+1</f>
         <v>27</v>
       </c>
       <c r="AD1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AD1" si="26">AC1+1</f>
         <v>28</v>
       </c>
       <c r="AE1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AE1" si="27">AD1+1</f>
         <v>29</v>
       </c>
       <c r="AF1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AF1" si="28">AE1+1</f>
         <v>30</v>
       </c>
       <c r="AG1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AG1" si="29">AF1+1</f>
         <v>31</v>
       </c>
       <c r="AH1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AH1" si="30">AG1+1</f>
         <v>32</v>
       </c>
       <c r="AI1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AI1" si="31">AH1+1</f>
         <v>33</v>
       </c>
       <c r="AJ1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AJ1" si="32">AI1+1</f>
         <v>34</v>
       </c>
       <c r="AK1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AK1" si="33">AJ1+1</f>
         <v>35</v>
       </c>
       <c r="AL1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AL1" si="34">AK1+1</f>
         <v>36</v>
       </c>
       <c r="AM1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AM1" si="35">AL1+1</f>
         <v>37</v>
       </c>
       <c r="AN1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AN1" si="36">AM1+1</f>
         <v>38</v>
       </c>
       <c r="AO1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AO1" si="37">AN1+1</f>
         <v>39</v>
       </c>
       <c r="AP1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AP1" si="38">AO1+1</f>
         <v>40</v>
       </c>
       <c r="AQ1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AQ1" si="39">AP1+1</f>
         <v>41</v>
       </c>
       <c r="AR1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AR1" si="40">AQ1+1</f>
         <v>42</v>
       </c>
       <c r="AS1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AS1" si="41">AR1+1</f>
         <v>43</v>
       </c>
       <c r="AT1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AT1" si="42">AS1+1</f>
         <v>44</v>
       </c>
       <c r="AU1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AU1" si="43">AT1+1</f>
         <v>45</v>
       </c>
       <c r="AV1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AV1" si="44">AU1+1</f>
         <v>46</v>
       </c>
       <c r="AW1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AW1" si="45">AV1+1</f>
         <v>47</v>
       </c>
       <c r="AX1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AX1" si="46">AW1+1</f>
         <v>48</v>
       </c>
       <c r="AY1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AY1" si="47">AX1+1</f>
         <v>49</v>
       </c>
       <c r="AZ1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AZ1" si="48">AY1+1</f>
         <v>50</v>
       </c>
       <c r="BA1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="BA1" si="49">AZ1+1</f>
         <v>51</v>
       </c>
       <c r="BB1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="BB1" si="50">BA1+1</f>
         <v>52</v>
       </c>
       <c r="BC1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="BC1" si="51">BB1+1</f>
         <v>53</v>
       </c>
       <c r="BD1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="BD1" si="52">BC1+1</f>
         <v>54</v>
       </c>
       <c r="BE1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="BE1" si="53">BD1+1</f>
         <v>55</v>
       </c>
       <c r="BF1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="BF1" si="54">BE1+1</f>
         <v>56</v>
       </c>
       <c r="BG1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="BG1" si="55">BF1+1</f>
         <v>57</v>
       </c>
       <c r="BH1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="BH1" si="56">BG1+1</f>
         <v>58</v>
       </c>
       <c r="BI1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="BI1" si="57">BH1+1</f>
         <v>59</v>
       </c>
       <c r="BJ1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="BJ1" si="58">BI1+1</f>
         <v>60</v>
       </c>
       <c r="BK1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="BK1" si="59">BJ1+1</f>
         <v>61</v>
       </c>
       <c r="BL1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="BL1" si="60">BK1+1</f>
         <v>62</v>
       </c>
       <c r="BM1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="BM1" si="61">BL1+1</f>
         <v>63</v>
       </c>
       <c r="BN1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="BN1" si="62">BM1+1</f>
         <v>64</v>
       </c>
       <c r="BO1" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="BO1" si="63">BN1+1</f>
         <v>65</v>
       </c>
       <c r="BP1" s="11">
-        <f t="shared" ref="BP1:BX1" si="1">BO1+1</f>
+        <f t="shared" ref="BP1" si="64">BO1+1</f>
         <v>66</v>
       </c>
       <c r="BQ1" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="BQ1" si="65">BP1+1</f>
         <v>67</v>
       </c>
       <c r="BR1" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="BR1" si="66">BQ1+1</f>
         <v>68</v>
       </c>
       <c r="BS1" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="BS1" si="67">BR1+1</f>
         <v>69</v>
       </c>
       <c r="BT1" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="BT1" si="68">BS1+1</f>
         <v>70</v>
       </c>
       <c r="BU1" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="BU1" si="69">BT1+1</f>
         <v>71</v>
       </c>
       <c r="BV1" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="BV1" si="70">BU1+1</f>
         <v>72</v>
       </c>
       <c r="BW1" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="BW1" si="71">BV1+1</f>
         <v>73</v>
       </c>
       <c r="BX1" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="BX1" si="72">BW1+1</f>
         <v>74</v>
       </c>
     </row>
@@ -842,14 +845,14 @@
       <c r="Q2" s="12"/>
       <c r="R2" s="12"/>
       <c r="S2" s="12"/>
-      <c r="T2" s="13"/>
-      <c r="U2" s="13"/>
-      <c r="V2" s="13"/>
-      <c r="W2" s="13"/>
-      <c r="X2" s="13"/>
-      <c r="Y2" s="13"/>
-      <c r="Z2" s="13"/>
-      <c r="AA2" s="13"/>
+      <c r="T2" s="12"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="12"/>
+      <c r="W2" s="12"/>
+      <c r="X2" s="12"/>
+      <c r="Y2" s="12"/>
+      <c r="Z2" s="12"/>
+      <c r="AA2" s="12"/>
       <c r="AB2" s="12"/>
       <c r="AC2" s="12"/>
       <c r="AD2" s="12"/>
@@ -923,13 +926,13 @@
       <c r="R3" s="12"/>
       <c r="S3" s="12"/>
       <c r="T3" s="13"/>
-      <c r="U3" s="13"/>
-      <c r="V3" s="13"/>
-      <c r="W3" s="13"/>
-      <c r="X3" s="13"/>
-      <c r="Y3" s="13"/>
-      <c r="Z3" s="13"/>
-      <c r="AA3" s="13"/>
+      <c r="U3" s="14"/>
+      <c r="V3" s="15"/>
+      <c r="W3" s="14"/>
+      <c r="X3" s="12"/>
+      <c r="Y3" s="12"/>
+      <c r="Z3" s="12"/>
+      <c r="AA3" s="12"/>
       <c r="AB3" s="12"/>
       <c r="AC3" s="12"/>
       <c r="AD3" s="12"/>
@@ -990,26 +993,26 @@
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="12"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="13"/>
-      <c r="V4" s="13"/>
-      <c r="W4" s="13"/>
-      <c r="X4" s="13"/>
-      <c r="Y4" s="13"/>
-      <c r="Z4" s="13"/>
-      <c r="AA4" s="13"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="14"/>
+      <c r="U4" s="12"/>
+      <c r="V4" s="12"/>
+      <c r="W4" s="12"/>
+      <c r="X4" s="14"/>
+      <c r="Y4" s="12"/>
+      <c r="Z4" s="12"/>
+      <c r="AA4" s="12"/>
       <c r="AB4" s="12"/>
       <c r="AC4" s="12"/>
       <c r="AD4" s="12"/>
@@ -1071,30 +1074,30 @@
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
-      <c r="I5" s="14"/>
+      <c r="I5" s="12"/>
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
-      <c r="M5" s="14"/>
+      <c r="M5" s="12"/>
       <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
+      <c r="O5" s="14"/>
       <c r="P5" s="12"/>
       <c r="Q5" s="12"/>
       <c r="R5" s="12"/>
       <c r="S5" s="12"/>
-      <c r="T5" s="13"/>
-      <c r="U5" s="13"/>
-      <c r="V5" s="13"/>
-      <c r="W5" s="13"/>
-      <c r="X5" s="13"/>
-      <c r="Y5" s="13"/>
-      <c r="Z5" s="13"/>
-      <c r="AA5" s="13"/>
+      <c r="T5" s="12"/>
+      <c r="U5" s="12"/>
+      <c r="V5" s="12"/>
+      <c r="W5" s="12"/>
+      <c r="X5" s="12"/>
+      <c r="Y5" s="14"/>
+      <c r="Z5" s="12"/>
+      <c r="AA5" s="12"/>
       <c r="AB5" s="12"/>
-      <c r="AC5" s="12"/>
-      <c r="AD5" s="12"/>
-      <c r="AE5" s="12"/>
-      <c r="AF5" s="12"/>
+      <c r="AC5" s="13"/>
+      <c r="AD5" s="14"/>
+      <c r="AE5" s="15"/>
+      <c r="AF5" s="14"/>
       <c r="AG5" s="12"/>
       <c r="AH5" s="12"/>
       <c r="AI5" s="12"/>
@@ -1151,8 +1154,8 @@
       <c r="F6" s="14"/>
       <c r="G6" s="15"/>
       <c r="H6" s="14"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
       <c r="M6" s="12"/>
@@ -1168,14 +1171,14 @@
       <c r="W6" s="13"/>
       <c r="X6" s="13"/>
       <c r="Y6" s="13"/>
-      <c r="Z6" s="13"/>
-      <c r="AA6" s="13"/>
-      <c r="AB6" s="12"/>
-      <c r="AC6" s="12"/>
+      <c r="Z6" s="14"/>
+      <c r="AA6" s="15"/>
+      <c r="AB6" s="14"/>
+      <c r="AC6" s="14"/>
       <c r="AD6" s="12"/>
       <c r="AE6" s="12"/>
       <c r="AF6" s="12"/>
-      <c r="AG6" s="12"/>
+      <c r="AG6" s="14"/>
       <c r="AH6" s="12"/>
       <c r="AI6" s="12"/>
       <c r="AJ6" s="12"/>
@@ -1230,16 +1233,16 @@
       <c r="E7" s="14"/>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
       <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="15"/>
-      <c r="Q7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
       <c r="R7" s="12"/>
       <c r="S7" s="12"/>
       <c r="T7" s="12"/>
@@ -1251,14 +1254,14 @@
       <c r="Z7" s="12"/>
       <c r="AA7" s="12"/>
       <c r="AB7" s="12"/>
-      <c r="AC7" s="12"/>
-      <c r="AD7" s="12"/>
-      <c r="AE7" s="12"/>
-      <c r="AF7" s="12"/>
-      <c r="AG7" s="12"/>
-      <c r="AH7" s="12"/>
-      <c r="AI7" s="12"/>
-      <c r="AJ7" s="12"/>
+      <c r="AC7" s="13"/>
+      <c r="AD7" s="13"/>
+      <c r="AE7" s="13"/>
+      <c r="AF7" s="13"/>
+      <c r="AG7" s="13"/>
+      <c r="AH7" s="14"/>
+      <c r="AI7" s="15"/>
+      <c r="AJ7" s="14"/>
       <c r="AK7" s="12"/>
       <c r="AL7" s="12"/>
       <c r="AM7" s="12"/>
@@ -1310,19 +1313,19 @@
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="13"/>
-      <c r="R8" s="14"/>
-      <c r="S8" s="15"/>
-      <c r="T8" s="14"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
+      <c r="S8" s="12"/>
+      <c r="T8" s="12"/>
       <c r="U8" s="12"/>
       <c r="V8" s="12"/>
       <c r="W8" s="12"/>
@@ -1403,7 +1406,7 @@
       <c r="R9" s="12"/>
       <c r="S9" s="12"/>
       <c r="T9" s="12"/>
-      <c r="U9" s="14"/>
+      <c r="U9" s="12"/>
       <c r="V9" s="12"/>
       <c r="W9" s="12"/>
       <c r="X9" s="12"/>
@@ -1482,9 +1485,9 @@
       <c r="Q10" s="12"/>
       <c r="R10" s="12"/>
       <c r="S10" s="12"/>
-      <c r="T10" s="13"/>
-      <c r="U10" s="13"/>
-      <c r="V10" s="14"/>
+      <c r="T10" s="12"/>
+      <c r="U10" s="12"/>
+      <c r="V10" s="12"/>
       <c r="W10" s="12"/>
       <c r="X10" s="12"/>
       <c r="Y10" s="12"/>
@@ -1542,7 +1545,7 @@
     </row>
     <row r="11" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B11" s="11">
         <v>0</v>
@@ -1552,295 +1555,295 @@
         <v>1</v>
       </c>
       <c r="D11" s="11">
-        <f t="shared" ref="D11:BO11" si="2">C11+1</f>
+        <f t="shared" ref="D11:BO11" si="73">C11+1</f>
         <v>2</v>
       </c>
       <c r="E11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>3</v>
       </c>
       <c r="F11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>4</v>
       </c>
       <c r="G11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>5</v>
       </c>
       <c r="H11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>6</v>
       </c>
       <c r="I11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>7</v>
       </c>
       <c r="J11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>8</v>
       </c>
       <c r="K11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>9</v>
       </c>
       <c r="L11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>10</v>
       </c>
       <c r="M11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>11</v>
       </c>
       <c r="N11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>12</v>
       </c>
       <c r="O11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>13</v>
       </c>
       <c r="P11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>14</v>
       </c>
       <c r="Q11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>15</v>
       </c>
       <c r="R11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>16</v>
       </c>
       <c r="S11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>17</v>
       </c>
       <c r="T11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>18</v>
       </c>
       <c r="U11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>19</v>
       </c>
       <c r="V11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>20</v>
       </c>
       <c r="W11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>21</v>
       </c>
       <c r="X11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>22</v>
       </c>
       <c r="Y11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>23</v>
       </c>
       <c r="Z11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>24</v>
       </c>
       <c r="AA11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>25</v>
       </c>
       <c r="AB11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>26</v>
       </c>
       <c r="AC11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>27</v>
       </c>
       <c r="AD11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>28</v>
       </c>
       <c r="AE11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>29</v>
       </c>
       <c r="AF11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>30</v>
       </c>
       <c r="AG11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>31</v>
       </c>
       <c r="AH11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>32</v>
       </c>
       <c r="AI11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>33</v>
       </c>
       <c r="AJ11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>34</v>
       </c>
       <c r="AK11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>35</v>
       </c>
       <c r="AL11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>36</v>
       </c>
       <c r="AM11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>37</v>
       </c>
       <c r="AN11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>38</v>
       </c>
       <c r="AO11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>39</v>
       </c>
       <c r="AP11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>40</v>
       </c>
       <c r="AQ11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>41</v>
       </c>
       <c r="AR11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>42</v>
       </c>
       <c r="AS11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>43</v>
       </c>
       <c r="AT11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>44</v>
       </c>
       <c r="AU11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>45</v>
       </c>
       <c r="AV11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>46</v>
       </c>
       <c r="AW11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>47</v>
       </c>
       <c r="AX11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>48</v>
       </c>
       <c r="AY11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>49</v>
       </c>
       <c r="AZ11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>50</v>
       </c>
       <c r="BA11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>51</v>
       </c>
       <c r="BB11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>52</v>
       </c>
       <c r="BC11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>53</v>
       </c>
       <c r="BD11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>54</v>
       </c>
       <c r="BE11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>55</v>
       </c>
       <c r="BF11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>56</v>
       </c>
       <c r="BG11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>57</v>
       </c>
       <c r="BH11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>58</v>
       </c>
       <c r="BI11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>59</v>
       </c>
       <c r="BJ11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>60</v>
       </c>
       <c r="BK11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>61</v>
       </c>
       <c r="BL11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>62</v>
       </c>
       <c r="BM11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>63</v>
       </c>
       <c r="BN11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>64</v>
       </c>
       <c r="BO11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="73"/>
         <v>65</v>
       </c>
       <c r="BP11" s="11">
-        <f t="shared" ref="BP11:BX11" si="3">BO11+1</f>
+        <f t="shared" ref="BP11:BX11" si="74">BO11+1</f>
         <v>66</v>
       </c>
       <c r="BQ11" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="74"/>
         <v>67</v>
       </c>
       <c r="BR11" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="74"/>
         <v>68</v>
       </c>
       <c r="BS11" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="74"/>
         <v>69</v>
       </c>
       <c r="BT11" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="74"/>
         <v>70</v>
       </c>
       <c r="BU11" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="74"/>
         <v>71</v>
       </c>
       <c r="BV11" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="74"/>
         <v>72</v>
       </c>
       <c r="BW11" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="74"/>
         <v>73</v>
       </c>
       <c r="BX11" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="74"/>
         <v>74</v>
       </c>
     </row>
@@ -1866,14 +1869,14 @@
       <c r="Q12" s="12"/>
       <c r="R12" s="12"/>
       <c r="S12" s="12"/>
-      <c r="T12" s="12"/>
-      <c r="U12" s="12"/>
-      <c r="V12" s="12"/>
-      <c r="W12" s="12"/>
-      <c r="X12" s="12"/>
-      <c r="Y12" s="12"/>
-      <c r="Z12" s="12"/>
-      <c r="AA12" s="12"/>
+      <c r="T12" s="13"/>
+      <c r="U12" s="13"/>
+      <c r="V12" s="13"/>
+      <c r="W12" s="13"/>
+      <c r="X12" s="13"/>
+      <c r="Y12" s="13"/>
+      <c r="Z12" s="13"/>
+      <c r="AA12" s="13"/>
       <c r="AB12" s="12"/>
       <c r="AC12" s="12"/>
       <c r="AD12" s="12"/>
@@ -1946,14 +1949,14 @@
       <c r="Q13" s="12"/>
       <c r="R13" s="12"/>
       <c r="S13" s="12"/>
-      <c r="T13" s="12"/>
-      <c r="U13" s="12"/>
-      <c r="V13" s="12"/>
-      <c r="W13" s="12"/>
-      <c r="X13" s="12"/>
-      <c r="Y13" s="12"/>
-      <c r="Z13" s="12"/>
-      <c r="AA13" s="12"/>
+      <c r="T13" s="13"/>
+      <c r="U13" s="13"/>
+      <c r="V13" s="13"/>
+      <c r="W13" s="13"/>
+      <c r="X13" s="13"/>
+      <c r="Y13" s="13"/>
+      <c r="Z13" s="13"/>
+      <c r="AA13" s="13"/>
       <c r="AB13" s="12"/>
       <c r="AC13" s="12"/>
       <c r="AD13" s="12"/>
@@ -2014,18 +2017,18 @@
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="14"/>
       <c r="M14" s="12"/>
       <c r="N14" s="12"/>
       <c r="O14" s="12"/>
       <c r="P14" s="12"/>
       <c r="Q14" s="12"/>
-      <c r="R14" s="13"/>
-      <c r="S14" s="13"/>
+      <c r="R14" s="12"/>
+      <c r="S14" s="12"/>
       <c r="T14" s="13"/>
       <c r="U14" s="13"/>
       <c r="V14" s="13"/>
@@ -2034,10 +2037,10 @@
       <c r="Y14" s="13"/>
       <c r="Z14" s="13"/>
       <c r="AA14" s="13"/>
-      <c r="AB14" s="13"/>
-      <c r="AC14" s="14"/>
-      <c r="AD14" s="15"/>
-      <c r="AE14" s="14"/>
+      <c r="AB14" s="12"/>
+      <c r="AC14" s="12"/>
+      <c r="AD14" s="12"/>
+      <c r="AE14" s="12"/>
       <c r="AF14" s="12"/>
       <c r="AG14" s="12"/>
       <c r="AH14" s="12"/>
@@ -2053,11 +2056,11 @@
       <c r="AR14" s="12"/>
       <c r="AS14" s="12"/>
       <c r="AT14" s="12"/>
-      <c r="AU14" s="13"/>
-      <c r="AV14" s="13"/>
-      <c r="AW14" s="14"/>
-      <c r="AX14" s="15"/>
-      <c r="AY14" s="14"/>
+      <c r="AU14" s="12"/>
+      <c r="AV14" s="12"/>
+      <c r="AW14" s="12"/>
+      <c r="AX14" s="12"/>
+      <c r="AY14" s="12"/>
       <c r="AZ14" s="12"/>
       <c r="BA14" s="12"/>
       <c r="BB14" s="12"/>
@@ -2095,30 +2098,30 @@
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
+      <c r="I15" s="14"/>
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
+      <c r="M15" s="14"/>
       <c r="N15" s="12"/>
       <c r="O15" s="12"/>
       <c r="P15" s="12"/>
       <c r="Q15" s="12"/>
       <c r="R15" s="12"/>
       <c r="S15" s="12"/>
-      <c r="T15" s="12"/>
-      <c r="U15" s="12"/>
-      <c r="V15" s="12"/>
-      <c r="W15" s="12"/>
-      <c r="X15" s="12"/>
-      <c r="Y15" s="12"/>
-      <c r="Z15" s="12"/>
-      <c r="AA15" s="12"/>
-      <c r="AB15" s="14"/>
+      <c r="T15" s="13"/>
+      <c r="U15" s="13"/>
+      <c r="V15" s="13"/>
+      <c r="W15" s="13"/>
+      <c r="X15" s="13"/>
+      <c r="Y15" s="13"/>
+      <c r="Z15" s="13"/>
+      <c r="AA15" s="13"/>
+      <c r="AB15" s="12"/>
       <c r="AC15" s="12"/>
       <c r="AD15" s="12"/>
       <c r="AE15" s="12"/>
-      <c r="AF15" s="14"/>
+      <c r="AF15" s="12"/>
       <c r="AG15" s="12"/>
       <c r="AH15" s="12"/>
       <c r="AI15" s="12"/>
@@ -2129,28 +2132,28 @@
       <c r="AN15" s="12"/>
       <c r="AO15" s="12"/>
       <c r="AP15" s="12"/>
-      <c r="AQ15" s="13"/>
-      <c r="AR15" s="13"/>
-      <c r="AS15" s="13"/>
-      <c r="AT15" s="14"/>
-      <c r="AU15" s="15"/>
-      <c r="AV15" s="14"/>
+      <c r="AQ15" s="12"/>
+      <c r="AR15" s="12"/>
+      <c r="AS15" s="12"/>
+      <c r="AT15" s="12"/>
+      <c r="AU15" s="12"/>
+      <c r="AV15" s="12"/>
       <c r="AW15" s="12"/>
       <c r="AX15" s="12"/>
       <c r="AY15" s="12"/>
-      <c r="AZ15" s="14"/>
+      <c r="AZ15" s="12"/>
       <c r="BA15" s="12"/>
-      <c r="BB15" s="13"/>
-      <c r="BC15" s="13"/>
-      <c r="BD15" s="13"/>
-      <c r="BE15" s="13"/>
-      <c r="BF15" s="13"/>
-      <c r="BG15" s="13"/>
-      <c r="BH15" s="13"/>
-      <c r="BI15" s="13"/>
-      <c r="BJ15" s="14"/>
-      <c r="BK15" s="15"/>
-      <c r="BL15" s="14"/>
+      <c r="BB15" s="12"/>
+      <c r="BC15" s="12"/>
+      <c r="BD15" s="12"/>
+      <c r="BE15" s="12"/>
+      <c r="BF15" s="12"/>
+      <c r="BG15" s="12"/>
+      <c r="BH15" s="12"/>
+      <c r="BI15" s="12"/>
+      <c r="BJ15" s="12"/>
+      <c r="BK15" s="12"/>
+      <c r="BL15" s="12"/>
       <c r="BM15" s="12"/>
       <c r="BN15" s="12"/>
       <c r="BO15" s="12"/>
@@ -2168,70 +2171,70 @@
       <c r="A16">
         <v>4</v>
       </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="14"/>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="14"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="12"/>
       <c r="P16" s="12"/>
       <c r="Q16" s="12"/>
       <c r="R16" s="12"/>
       <c r="S16" s="12"/>
-      <c r="T16" s="12"/>
-      <c r="U16" s="12"/>
-      <c r="V16" s="12"/>
-      <c r="W16" s="12"/>
-      <c r="X16" s="12"/>
-      <c r="Y16" s="12"/>
-      <c r="Z16" s="12"/>
-      <c r="AA16" s="14"/>
+      <c r="T16" s="13"/>
+      <c r="U16" s="13"/>
+      <c r="V16" s="13"/>
+      <c r="W16" s="13"/>
+      <c r="X16" s="13"/>
+      <c r="Y16" s="13"/>
+      <c r="Z16" s="13"/>
+      <c r="AA16" s="13"/>
       <c r="AB16" s="12"/>
       <c r="AC16" s="12"/>
       <c r="AD16" s="12"/>
       <c r="AE16" s="12"/>
       <c r="AF16" s="12"/>
-      <c r="AG16" s="14"/>
-      <c r="AH16" s="13"/>
-      <c r="AI16" s="13"/>
-      <c r="AJ16" s="13"/>
-      <c r="AK16" s="13"/>
-      <c r="AL16" s="13"/>
-      <c r="AM16" s="13"/>
-      <c r="AN16" s="13"/>
-      <c r="AO16" s="13"/>
-      <c r="AP16" s="13"/>
-      <c r="AQ16" s="14"/>
-      <c r="AR16" s="15"/>
-      <c r="AS16" s="14"/>
+      <c r="AG16" s="12"/>
+      <c r="AH16" s="12"/>
+      <c r="AI16" s="12"/>
+      <c r="AJ16" s="12"/>
+      <c r="AK16" s="12"/>
+      <c r="AL16" s="12"/>
+      <c r="AM16" s="12"/>
+      <c r="AN16" s="12"/>
+      <c r="AO16" s="12"/>
+      <c r="AP16" s="12"/>
+      <c r="AQ16" s="12"/>
+      <c r="AR16" s="12"/>
+      <c r="AS16" s="12"/>
       <c r="AT16" s="12"/>
-      <c r="AU16" s="13"/>
-      <c r="AV16" s="13"/>
-      <c r="AW16" s="13"/>
-      <c r="AX16" s="13"/>
-      <c r="AY16" s="13"/>
-      <c r="AZ16" s="13"/>
-      <c r="BA16" s="14"/>
-      <c r="BB16" s="15"/>
-      <c r="BC16" s="14"/>
+      <c r="AU16" s="12"/>
+      <c r="AV16" s="12"/>
+      <c r="AW16" s="12"/>
+      <c r="AX16" s="12"/>
+      <c r="AY16" s="12"/>
+      <c r="AZ16" s="12"/>
+      <c r="BA16" s="12"/>
+      <c r="BB16" s="12"/>
+      <c r="BC16" s="12"/>
       <c r="BD16" s="12"/>
       <c r="BE16" s="12"/>
       <c r="BF16" s="12"/>
-      <c r="BG16" s="14"/>
-      <c r="BH16" s="15"/>
-      <c r="BI16" s="14"/>
+      <c r="BG16" s="12"/>
+      <c r="BH16" s="12"/>
+      <c r="BI16" s="12"/>
       <c r="BJ16" s="12"/>
       <c r="BK16" s="12"/>
       <c r="BL16" s="12"/>
-      <c r="BM16" s="14"/>
+      <c r="BM16" s="12"/>
       <c r="BN16" s="12"/>
       <c r="BO16" s="12"/>
       <c r="BP16" s="12"/>
@@ -2251,19 +2254,19 @@
       <c r="B17" s="12"/>
       <c r="C17" s="12"/>
       <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
+      <c r="E17" s="14"/>
       <c r="F17" s="12"/>
       <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
-      <c r="O17" s="12"/>
-      <c r="P17" s="14"/>
-      <c r="Q17" s="12"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="14"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="14"/>
       <c r="R17" s="12"/>
       <c r="S17" s="12"/>
       <c r="T17" s="12"/>
@@ -2272,39 +2275,39 @@
       <c r="W17" s="12"/>
       <c r="X17" s="12"/>
       <c r="Y17" s="12"/>
-      <c r="Z17" s="14"/>
+      <c r="Z17" s="12"/>
       <c r="AA17" s="12"/>
       <c r="AB17" s="12"/>
       <c r="AC17" s="12"/>
       <c r="AD17" s="12"/>
-      <c r="AE17" s="13"/>
-      <c r="AF17" s="13"/>
-      <c r="AG17" s="13"/>
-      <c r="AH17" s="14"/>
-      <c r="AI17" s="15"/>
-      <c r="AJ17" s="14"/>
+      <c r="AE17" s="12"/>
+      <c r="AF17" s="12"/>
+      <c r="AG17" s="12"/>
+      <c r="AH17" s="12"/>
+      <c r="AI17" s="12"/>
+      <c r="AJ17" s="12"/>
       <c r="AK17" s="12"/>
       <c r="AL17" s="12"/>
       <c r="AM17" s="12"/>
       <c r="AN17" s="12"/>
       <c r="AO17" s="12"/>
-      <c r="AP17" s="14"/>
-      <c r="AQ17" s="13"/>
-      <c r="AR17" s="13"/>
-      <c r="AS17" s="13"/>
-      <c r="AT17" s="13"/>
-      <c r="AU17" s="13"/>
-      <c r="AV17" s="13"/>
-      <c r="AW17" s="13"/>
-      <c r="AX17" s="13"/>
-      <c r="AY17" s="13"/>
-      <c r="AZ17" s="13"/>
-      <c r="BA17" s="13"/>
-      <c r="BB17" s="13"/>
-      <c r="BC17" s="13"/>
-      <c r="BD17" s="14"/>
-      <c r="BE17" s="15"/>
-      <c r="BF17" s="14"/>
+      <c r="AP17" s="12"/>
+      <c r="AQ17" s="12"/>
+      <c r="AR17" s="12"/>
+      <c r="AS17" s="12"/>
+      <c r="AT17" s="12"/>
+      <c r="AU17" s="12"/>
+      <c r="AV17" s="12"/>
+      <c r="AW17" s="12"/>
+      <c r="AX17" s="12"/>
+      <c r="AY17" s="12"/>
+      <c r="AZ17" s="12"/>
+      <c r="BA17" s="12"/>
+      <c r="BB17" s="12"/>
+      <c r="BC17" s="12"/>
+      <c r="BD17" s="12"/>
+      <c r="BE17" s="12"/>
+      <c r="BF17" s="12"/>
       <c r="BG17" s="12"/>
       <c r="BH17" s="12"/>
       <c r="BI17" s="12"/>
@@ -2312,9 +2315,9 @@
       <c r="BK17" s="12"/>
       <c r="BL17" s="12"/>
       <c r="BM17" s="12"/>
-      <c r="BN17" s="14"/>
-      <c r="BO17" s="15"/>
-      <c r="BP17" s="14"/>
+      <c r="BN17" s="12"/>
+      <c r="BO17" s="12"/>
+      <c r="BP17" s="12"/>
       <c r="BQ17" s="12"/>
       <c r="BR17" s="12"/>
       <c r="BS17" s="12"/>
@@ -2330,28 +2333,28 @@
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
+      <c r="D18" s="14"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
       <c r="H18" s="13"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="12"/>
-      <c r="O18" s="12"/>
-      <c r="P18" s="12"/>
-      <c r="Q18" s="14"/>
-      <c r="R18" s="12"/>
-      <c r="S18" s="12"/>
-      <c r="T18" s="12"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="13"/>
+      <c r="P18" s="13"/>
+      <c r="Q18" s="13"/>
+      <c r="R18" s="14"/>
+      <c r="S18" s="15"/>
+      <c r="T18" s="14"/>
       <c r="U18" s="12"/>
       <c r="V18" s="12"/>
       <c r="W18" s="12"/>
       <c r="X18" s="12"/>
-      <c r="Y18" s="14"/>
+      <c r="Y18" s="12"/>
       <c r="Z18" s="12"/>
       <c r="AA18" s="12"/>
       <c r="AB18" s="12"/>
@@ -2363,11 +2366,11 @@
       <c r="AH18" s="12"/>
       <c r="AI18" s="12"/>
       <c r="AJ18" s="12"/>
-      <c r="AK18" s="14"/>
+      <c r="AK18" s="12"/>
       <c r="AL18" s="12"/>
       <c r="AM18" s="12"/>
       <c r="AN18" s="12"/>
-      <c r="AO18" s="14"/>
+      <c r="AO18" s="12"/>
       <c r="AP18" s="12"/>
       <c r="AQ18" s="12"/>
       <c r="AR18" s="12"/>
@@ -2390,14 +2393,14 @@
       <c r="BI18" s="12"/>
       <c r="BJ18" s="12"/>
       <c r="BK18" s="12"/>
-      <c r="BL18" s="13"/>
-      <c r="BM18" s="13"/>
-      <c r="BN18" s="13"/>
-      <c r="BO18" s="13"/>
-      <c r="BP18" s="13"/>
-      <c r="BQ18" s="14"/>
-      <c r="BR18" s="15"/>
-      <c r="BS18" s="14"/>
+      <c r="BL18" s="12"/>
+      <c r="BM18" s="12"/>
+      <c r="BN18" s="12"/>
+      <c r="BO18" s="12"/>
+      <c r="BP18" s="12"/>
+      <c r="BQ18" s="12"/>
+      <c r="BR18" s="12"/>
+      <c r="BS18" s="12"/>
       <c r="BT18" s="12"/>
       <c r="BU18" s="12"/>
       <c r="BV18" s="12"/>
@@ -2409,28 +2412,28 @@
         <v>1</v>
       </c>
       <c r="B19" s="12"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="13"/>
-      <c r="P19" s="13"/>
-      <c r="Q19" s="13"/>
-      <c r="R19" s="14"/>
-      <c r="S19" s="15"/>
-      <c r="T19" s="14"/>
-      <c r="U19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="12"/>
+      <c r="S19" s="12"/>
+      <c r="T19" s="12"/>
+      <c r="U19" s="14"/>
       <c r="V19" s="12"/>
       <c r="W19" s="12"/>
-      <c r="X19" s="14"/>
+      <c r="X19" s="12"/>
       <c r="Y19" s="12"/>
       <c r="Z19" s="12"/>
       <c r="AA19" s="12"/>
@@ -2440,13 +2443,13 @@
       <c r="AE19" s="12"/>
       <c r="AF19" s="12"/>
       <c r="AG19" s="12"/>
-      <c r="AH19" s="13"/>
-      <c r="AI19" s="13"/>
-      <c r="AJ19" s="13"/>
-      <c r="AK19" s="13"/>
-      <c r="AL19" s="14"/>
-      <c r="AM19" s="15"/>
-      <c r="AN19" s="14"/>
+      <c r="AH19" s="12"/>
+      <c r="AI19" s="12"/>
+      <c r="AJ19" s="12"/>
+      <c r="AK19" s="12"/>
+      <c r="AL19" s="12"/>
+      <c r="AM19" s="12"/>
+      <c r="AN19" s="12"/>
       <c r="AO19" s="12"/>
       <c r="AP19" s="12"/>
       <c r="AQ19" s="12"/>
@@ -2489,7 +2492,7 @@
         <v>0</v>
       </c>
       <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
+      <c r="C20" s="12"/>
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
@@ -2504,12 +2507,12 @@
       <c r="O20" s="12"/>
       <c r="P20" s="12"/>
       <c r="Q20" s="12"/>
-      <c r="R20" s="13"/>
-      <c r="S20" s="13"/>
+      <c r="R20" s="12"/>
+      <c r="S20" s="12"/>
       <c r="T20" s="13"/>
-      <c r="U20" s="14"/>
-      <c r="V20" s="15"/>
-      <c r="W20" s="14"/>
+      <c r="U20" s="13"/>
+      <c r="V20" s="14"/>
+      <c r="W20" s="12"/>
       <c r="X20" s="12"/>
       <c r="Y20" s="12"/>
       <c r="Z20" s="12"/>
@@ -2565,298 +2568,1098 @@
       <c r="BX20" s="12"/>
     </row>
     <row r="21" spans="1:76" x14ac:dyDescent="0.25">
-      <c r="D21"/>
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="11">
+        <v>0</v>
+      </c>
+      <c r="C21" s="11">
+        <f>B21+1</f>
+        <v>1</v>
+      </c>
+      <c r="D21" s="11">
+        <f t="shared" ref="D21:BO21" si="75">C21+1</f>
+        <v>2</v>
+      </c>
+      <c r="E21" s="11">
+        <f t="shared" si="75"/>
+        <v>3</v>
+      </c>
+      <c r="F21" s="11">
+        <f t="shared" si="75"/>
+        <v>4</v>
+      </c>
+      <c r="G21" s="11">
+        <f t="shared" si="75"/>
+        <v>5</v>
+      </c>
+      <c r="H21" s="11">
+        <f t="shared" si="75"/>
+        <v>6</v>
+      </c>
+      <c r="I21" s="11">
+        <f t="shared" si="75"/>
+        <v>7</v>
+      </c>
+      <c r="J21" s="11">
+        <f t="shared" si="75"/>
+        <v>8</v>
+      </c>
+      <c r="K21" s="11">
+        <f t="shared" si="75"/>
+        <v>9</v>
+      </c>
+      <c r="L21" s="11">
+        <f t="shared" si="75"/>
+        <v>10</v>
+      </c>
+      <c r="M21" s="11">
+        <f t="shared" si="75"/>
+        <v>11</v>
+      </c>
+      <c r="N21" s="11">
+        <f t="shared" si="75"/>
+        <v>12</v>
+      </c>
+      <c r="O21" s="11">
+        <f t="shared" si="75"/>
+        <v>13</v>
+      </c>
+      <c r="P21" s="11">
+        <f t="shared" si="75"/>
+        <v>14</v>
+      </c>
+      <c r="Q21" s="11">
+        <f t="shared" si="75"/>
+        <v>15</v>
+      </c>
+      <c r="R21" s="11">
+        <f t="shared" si="75"/>
+        <v>16</v>
+      </c>
+      <c r="S21" s="11">
+        <f t="shared" si="75"/>
+        <v>17</v>
+      </c>
+      <c r="T21" s="11">
+        <f t="shared" si="75"/>
+        <v>18</v>
+      </c>
+      <c r="U21" s="11">
+        <f t="shared" si="75"/>
+        <v>19</v>
+      </c>
+      <c r="V21" s="11">
+        <f t="shared" si="75"/>
+        <v>20</v>
+      </c>
+      <c r="W21" s="11">
+        <f t="shared" si="75"/>
+        <v>21</v>
+      </c>
+      <c r="X21" s="11">
+        <f t="shared" si="75"/>
+        <v>22</v>
+      </c>
+      <c r="Y21" s="11">
+        <f t="shared" si="75"/>
+        <v>23</v>
+      </c>
+      <c r="Z21" s="11">
+        <f t="shared" si="75"/>
+        <v>24</v>
+      </c>
+      <c r="AA21" s="11">
+        <f t="shared" si="75"/>
+        <v>25</v>
+      </c>
+      <c r="AB21" s="11">
+        <f t="shared" si="75"/>
+        <v>26</v>
+      </c>
+      <c r="AC21" s="11">
+        <f t="shared" si="75"/>
+        <v>27</v>
+      </c>
+      <c r="AD21" s="11">
+        <f t="shared" si="75"/>
+        <v>28</v>
+      </c>
+      <c r="AE21" s="11">
+        <f t="shared" si="75"/>
+        <v>29</v>
+      </c>
+      <c r="AF21" s="11">
+        <f t="shared" si="75"/>
+        <v>30</v>
+      </c>
+      <c r="AG21" s="11">
+        <f t="shared" si="75"/>
+        <v>31</v>
+      </c>
+      <c r="AH21" s="11">
+        <f t="shared" si="75"/>
+        <v>32</v>
+      </c>
+      <c r="AI21" s="11">
+        <f t="shared" si="75"/>
+        <v>33</v>
+      </c>
+      <c r="AJ21" s="11">
+        <f t="shared" si="75"/>
+        <v>34</v>
+      </c>
+      <c r="AK21" s="11">
+        <f t="shared" si="75"/>
+        <v>35</v>
+      </c>
+      <c r="AL21" s="11">
+        <f t="shared" si="75"/>
+        <v>36</v>
+      </c>
+      <c r="AM21" s="11">
+        <f t="shared" si="75"/>
+        <v>37</v>
+      </c>
+      <c r="AN21" s="11">
+        <f t="shared" si="75"/>
+        <v>38</v>
+      </c>
+      <c r="AO21" s="11">
+        <f t="shared" si="75"/>
+        <v>39</v>
+      </c>
+      <c r="AP21" s="11">
+        <f t="shared" si="75"/>
+        <v>40</v>
+      </c>
+      <c r="AQ21" s="11">
+        <f t="shared" si="75"/>
+        <v>41</v>
+      </c>
+      <c r="AR21" s="11">
+        <f t="shared" si="75"/>
+        <v>42</v>
+      </c>
+      <c r="AS21" s="11">
+        <f t="shared" si="75"/>
+        <v>43</v>
+      </c>
+      <c r="AT21" s="11">
+        <f t="shared" si="75"/>
+        <v>44</v>
+      </c>
+      <c r="AU21" s="11">
+        <f t="shared" si="75"/>
+        <v>45</v>
+      </c>
+      <c r="AV21" s="11">
+        <f t="shared" si="75"/>
+        <v>46</v>
+      </c>
+      <c r="AW21" s="11">
+        <f t="shared" si="75"/>
+        <v>47</v>
+      </c>
+      <c r="AX21" s="11">
+        <f t="shared" si="75"/>
+        <v>48</v>
+      </c>
+      <c r="AY21" s="11">
+        <f t="shared" si="75"/>
+        <v>49</v>
+      </c>
+      <c r="AZ21" s="11">
+        <f t="shared" si="75"/>
+        <v>50</v>
+      </c>
+      <c r="BA21" s="11">
+        <f t="shared" si="75"/>
+        <v>51</v>
+      </c>
+      <c r="BB21" s="11">
+        <f t="shared" si="75"/>
+        <v>52</v>
+      </c>
+      <c r="BC21" s="11">
+        <f t="shared" si="75"/>
+        <v>53</v>
+      </c>
+      <c r="BD21" s="11">
+        <f t="shared" si="75"/>
+        <v>54</v>
+      </c>
+      <c r="BE21" s="11">
+        <f t="shared" si="75"/>
+        <v>55</v>
+      </c>
+      <c r="BF21" s="11">
+        <f t="shared" si="75"/>
+        <v>56</v>
+      </c>
+      <c r="BG21" s="11">
+        <f t="shared" si="75"/>
+        <v>57</v>
+      </c>
+      <c r="BH21" s="11">
+        <f t="shared" si="75"/>
+        <v>58</v>
+      </c>
+      <c r="BI21" s="11">
+        <f t="shared" si="75"/>
+        <v>59</v>
+      </c>
+      <c r="BJ21" s="11">
+        <f t="shared" si="75"/>
+        <v>60</v>
+      </c>
+      <c r="BK21" s="11">
+        <f t="shared" si="75"/>
+        <v>61</v>
+      </c>
+      <c r="BL21" s="11">
+        <f t="shared" si="75"/>
+        <v>62</v>
+      </c>
+      <c r="BM21" s="11">
+        <f t="shared" si="75"/>
+        <v>63</v>
+      </c>
+      <c r="BN21" s="11">
+        <f t="shared" si="75"/>
+        <v>64</v>
+      </c>
+      <c r="BO21" s="11">
+        <f t="shared" si="75"/>
+        <v>65</v>
+      </c>
+      <c r="BP21" s="11">
+        <f t="shared" ref="BP21:BX21" si="76">BO21+1</f>
+        <v>66</v>
+      </c>
+      <c r="BQ21" s="11">
+        <f t="shared" si="76"/>
+        <v>67</v>
+      </c>
+      <c r="BR21" s="11">
+        <f t="shared" si="76"/>
+        <v>68</v>
+      </c>
+      <c r="BS21" s="11">
+        <f t="shared" si="76"/>
+        <v>69</v>
+      </c>
+      <c r="BT21" s="11">
+        <f t="shared" si="76"/>
+        <v>70</v>
+      </c>
+      <c r="BU21" s="11">
+        <f t="shared" si="76"/>
+        <v>71</v>
+      </c>
+      <c r="BV21" s="11">
+        <f t="shared" si="76"/>
+        <v>72</v>
+      </c>
+      <c r="BW21" s="11">
+        <f t="shared" si="76"/>
+        <v>73</v>
+      </c>
+      <c r="BX21" s="11">
+        <f t="shared" si="76"/>
+        <v>74</v>
+      </c>
     </row>
     <row r="22" spans="1:76" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22">
-        <v>2</v>
-      </c>
-      <c r="E22">
-        <v>3</v>
-      </c>
-      <c r="F22">
-        <v>4</v>
-      </c>
-      <c r="G22">
-        <v>5</v>
-      </c>
-      <c r="H22">
-        <v>6</v>
-      </c>
-      <c r="I22">
-        <v>7</v>
-      </c>
-      <c r="J22">
+      <c r="A22">
         <v>8</v>
       </c>
-      <c r="K22">
-        <v>9</v>
-      </c>
-      <c r="L22">
-        <v>10</v>
-      </c>
-      <c r="M22">
-        <v>11</v>
-      </c>
-      <c r="N22">
-        <v>12</v>
-      </c>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="12"/>
+      <c r="R22" s="12"/>
+      <c r="S22" s="12"/>
+      <c r="T22" s="12"/>
+      <c r="U22" s="12"/>
+      <c r="V22" s="12"/>
+      <c r="W22" s="12"/>
+      <c r="X22" s="12"/>
+      <c r="Y22" s="12"/>
+      <c r="Z22" s="12"/>
+      <c r="AA22" s="12"/>
+      <c r="AB22" s="12"/>
+      <c r="AC22" s="12"/>
+      <c r="AD22" s="12"/>
+      <c r="AE22" s="12"/>
+      <c r="AF22" s="12"/>
+      <c r="AG22" s="12"/>
+      <c r="AH22" s="12"/>
+      <c r="AI22" s="12"/>
+      <c r="AJ22" s="12"/>
+      <c r="AK22" s="12"/>
+      <c r="AL22" s="12"/>
+      <c r="AM22" s="12"/>
+      <c r="AN22" s="12"/>
+      <c r="AO22" s="12"/>
+      <c r="AP22" s="12"/>
+      <c r="AQ22" s="12"/>
+      <c r="AR22" s="12"/>
+      <c r="AS22" s="12"/>
+      <c r="AT22" s="12"/>
+      <c r="AU22" s="12"/>
+      <c r="AV22" s="12"/>
+      <c r="AW22" s="12"/>
+      <c r="AX22" s="12"/>
+      <c r="AY22" s="12"/>
+      <c r="AZ22" s="12"/>
+      <c r="BA22" s="12"/>
+      <c r="BB22" s="12"/>
+      <c r="BC22" s="12"/>
+      <c r="BD22" s="12"/>
+      <c r="BE22" s="12"/>
+      <c r="BF22" s="12"/>
+      <c r="BG22" s="12"/>
+      <c r="BH22" s="12"/>
+      <c r="BI22" s="12"/>
+      <c r="BJ22" s="12"/>
+      <c r="BK22" s="12"/>
+      <c r="BL22" s="12"/>
+      <c r="BM22" s="12"/>
+      <c r="BN22" s="12"/>
+      <c r="BO22" s="12"/>
+      <c r="BP22" s="12"/>
+      <c r="BQ22" s="12"/>
+      <c r="BR22" s="12"/>
+      <c r="BS22" s="12"/>
+      <c r="BT22" s="12"/>
+      <c r="BU22" s="12"/>
+      <c r="BV22" s="12"/>
+      <c r="BW22" s="12"/>
+      <c r="BX22" s="12"/>
     </row>
     <row r="23" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>8</v>
-      </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+      <c r="P23" s="12"/>
+      <c r="Q23" s="12"/>
+      <c r="R23" s="12"/>
+      <c r="S23" s="12"/>
+      <c r="T23" s="12"/>
+      <c r="U23" s="12"/>
+      <c r="V23" s="12"/>
+      <c r="W23" s="12"/>
+      <c r="X23" s="12"/>
+      <c r="Y23" s="12"/>
+      <c r="Z23" s="12"/>
+      <c r="AA23" s="12"/>
+      <c r="AB23" s="12"/>
+      <c r="AC23" s="12"/>
+      <c r="AD23" s="12"/>
+      <c r="AE23" s="12"/>
+      <c r="AF23" s="12"/>
+      <c r="AG23" s="12"/>
+      <c r="AH23" s="12"/>
+      <c r="AI23" s="12"/>
+      <c r="AJ23" s="12"/>
+      <c r="AK23" s="12"/>
+      <c r="AL23" s="12"/>
+      <c r="AM23" s="12"/>
+      <c r="AN23" s="12"/>
+      <c r="AO23" s="12"/>
+      <c r="AP23" s="12"/>
+      <c r="AQ23" s="12"/>
+      <c r="AR23" s="12"/>
+      <c r="AS23" s="12"/>
+      <c r="AT23" s="12"/>
+      <c r="AU23" s="12"/>
+      <c r="AV23" s="12"/>
+      <c r="AW23" s="12"/>
+      <c r="AX23" s="12"/>
+      <c r="AY23" s="12"/>
+      <c r="AZ23" s="12"/>
+      <c r="BA23" s="12"/>
+      <c r="BB23" s="12"/>
+      <c r="BC23" s="12"/>
+      <c r="BD23" s="12"/>
+      <c r="BE23" s="12"/>
+      <c r="BF23" s="12"/>
+      <c r="BG23" s="12"/>
+      <c r="BH23" s="12"/>
+      <c r="BI23" s="12"/>
+      <c r="BJ23" s="12"/>
+      <c r="BK23" s="12"/>
+      <c r="BL23" s="12"/>
+      <c r="BM23" s="12"/>
+      <c r="BN23" s="12"/>
+      <c r="BO23" s="12"/>
+      <c r="BP23" s="12"/>
+      <c r="BQ23" s="12"/>
+      <c r="BR23" s="12"/>
+      <c r="BS23" s="12"/>
+      <c r="BT23" s="12"/>
+      <c r="BU23" s="12"/>
+      <c r="BV23" s="12"/>
+      <c r="BW23" s="12"/>
+      <c r="BX23" s="12"/>
     </row>
     <row r="24" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>7</v>
-      </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="12"/>
+      <c r="P24" s="12"/>
+      <c r="Q24" s="12"/>
+      <c r="R24" s="13"/>
+      <c r="S24" s="13"/>
+      <c r="T24" s="13"/>
+      <c r="U24" s="13"/>
+      <c r="V24" s="13"/>
+      <c r="W24" s="13"/>
+      <c r="X24" s="13"/>
+      <c r="Y24" s="13"/>
+      <c r="Z24" s="13"/>
+      <c r="AA24" s="13"/>
+      <c r="AB24" s="13"/>
+      <c r="AC24" s="14"/>
+      <c r="AD24" s="15"/>
+      <c r="AE24" s="14"/>
+      <c r="AF24" s="12"/>
+      <c r="AG24" s="12"/>
+      <c r="AH24" s="12"/>
+      <c r="AI24" s="12"/>
+      <c r="AJ24" s="12"/>
+      <c r="AK24" s="12"/>
+      <c r="AL24" s="12"/>
+      <c r="AM24" s="12"/>
+      <c r="AN24" s="12"/>
+      <c r="AO24" s="12"/>
+      <c r="AP24" s="12"/>
+      <c r="AQ24" s="12"/>
+      <c r="AR24" s="12"/>
+      <c r="AS24" s="12"/>
+      <c r="AT24" s="12"/>
+      <c r="AU24" s="13"/>
+      <c r="AV24" s="13"/>
+      <c r="AW24" s="14"/>
+      <c r="AX24" s="15"/>
+      <c r="AY24" s="14"/>
+      <c r="AZ24" s="12"/>
+      <c r="BA24" s="12"/>
+      <c r="BB24" s="12"/>
+      <c r="BC24" s="12"/>
+      <c r="BD24" s="12"/>
+      <c r="BE24" s="12"/>
+      <c r="BF24" s="12"/>
+      <c r="BG24" s="12"/>
+      <c r="BH24" s="12"/>
+      <c r="BI24" s="12"/>
+      <c r="BJ24" s="12"/>
+      <c r="BK24" s="12"/>
+      <c r="BL24" s="12"/>
+      <c r="BM24" s="12"/>
+      <c r="BN24" s="12"/>
+      <c r="BO24" s="12"/>
+      <c r="BP24" s="12"/>
+      <c r="BQ24" s="12"/>
+      <c r="BR24" s="12"/>
+      <c r="BS24" s="12"/>
+      <c r="BT24" s="12"/>
+      <c r="BU24" s="12"/>
+      <c r="BV24" s="12"/>
+      <c r="BW24" s="12"/>
+      <c r="BX24" s="12"/>
     </row>
     <row r="25" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>6</v>
-      </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="12"/>
+      <c r="Q25" s="12"/>
+      <c r="R25" s="12"/>
+      <c r="S25" s="12"/>
+      <c r="T25" s="12"/>
+      <c r="U25" s="12"/>
+      <c r="V25" s="12"/>
+      <c r="W25" s="12"/>
+      <c r="X25" s="12"/>
+      <c r="Y25" s="12"/>
+      <c r="Z25" s="12"/>
+      <c r="AA25" s="12"/>
+      <c r="AB25" s="14"/>
+      <c r="AC25" s="12"/>
+      <c r="AD25" s="12"/>
+      <c r="AE25" s="12"/>
+      <c r="AF25" s="14"/>
+      <c r="AG25" s="12"/>
+      <c r="AH25" s="12"/>
+      <c r="AI25" s="12"/>
+      <c r="AJ25" s="12"/>
+      <c r="AK25" s="12"/>
+      <c r="AL25" s="12"/>
+      <c r="AM25" s="12"/>
+      <c r="AN25" s="12"/>
+      <c r="AO25" s="12"/>
+      <c r="AP25" s="12"/>
+      <c r="AQ25" s="13"/>
+      <c r="AR25" s="13"/>
+      <c r="AS25" s="13"/>
+      <c r="AT25" s="14"/>
+      <c r="AU25" s="15"/>
+      <c r="AV25" s="14"/>
+      <c r="AW25" s="12"/>
+      <c r="AX25" s="12"/>
+      <c r="AY25" s="12"/>
+      <c r="AZ25" s="14"/>
+      <c r="BA25" s="12"/>
+      <c r="BB25" s="13"/>
+      <c r="BC25" s="13"/>
+      <c r="BD25" s="13"/>
+      <c r="BE25" s="13"/>
+      <c r="BF25" s="13"/>
+      <c r="BG25" s="13"/>
+      <c r="BH25" s="13"/>
+      <c r="BI25" s="13"/>
+      <c r="BJ25" s="14"/>
+      <c r="BK25" s="15"/>
+      <c r="BL25" s="14"/>
+      <c r="BM25" s="12"/>
+      <c r="BN25" s="12"/>
+      <c r="BO25" s="12"/>
+      <c r="BP25" s="12"/>
+      <c r="BQ25" s="12"/>
+      <c r="BR25" s="12"/>
+      <c r="BS25" s="12"/>
+      <c r="BT25" s="12"/>
+      <c r="BU25" s="12"/>
+      <c r="BV25" s="12"/>
+      <c r="BW25" s="12"/>
+      <c r="BX25" s="12"/>
     </row>
     <row r="26" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>5</v>
-      </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="15"/>
+      <c r="O26" s="14"/>
+      <c r="P26" s="12"/>
+      <c r="Q26" s="12"/>
+      <c r="R26" s="12"/>
+      <c r="S26" s="12"/>
+      <c r="T26" s="12"/>
+      <c r="U26" s="12"/>
+      <c r="V26" s="12"/>
+      <c r="W26" s="12"/>
+      <c r="X26" s="12"/>
+      <c r="Y26" s="12"/>
+      <c r="Z26" s="12"/>
+      <c r="AA26" s="14"/>
+      <c r="AB26" s="12"/>
+      <c r="AC26" s="12"/>
+      <c r="AD26" s="12"/>
+      <c r="AE26" s="12"/>
+      <c r="AF26" s="12"/>
+      <c r="AG26" s="14"/>
+      <c r="AH26" s="13"/>
+      <c r="AI26" s="13"/>
+      <c r="AJ26" s="13"/>
+      <c r="AK26" s="13"/>
+      <c r="AL26" s="13"/>
+      <c r="AM26" s="13"/>
+      <c r="AN26" s="13"/>
+      <c r="AO26" s="13"/>
+      <c r="AP26" s="13"/>
+      <c r="AQ26" s="14"/>
+      <c r="AR26" s="15"/>
+      <c r="AS26" s="14"/>
+      <c r="AT26" s="12"/>
+      <c r="AU26" s="13"/>
+      <c r="AV26" s="13"/>
+      <c r="AW26" s="13"/>
+      <c r="AX26" s="13"/>
+      <c r="AY26" s="13"/>
+      <c r="AZ26" s="13"/>
+      <c r="BA26" s="14"/>
+      <c r="BB26" s="15"/>
+      <c r="BC26" s="14"/>
+      <c r="BD26" s="12"/>
+      <c r="BE26" s="12"/>
+      <c r="BF26" s="12"/>
+      <c r="BG26" s="14"/>
+      <c r="BH26" s="15"/>
+      <c r="BI26" s="14"/>
+      <c r="BJ26" s="12"/>
+      <c r="BK26" s="12"/>
+      <c r="BL26" s="12"/>
+      <c r="BM26" s="14"/>
+      <c r="BN26" s="12"/>
+      <c r="BO26" s="12"/>
+      <c r="BP26" s="12"/>
+      <c r="BQ26" s="12"/>
+      <c r="BR26" s="12"/>
+      <c r="BS26" s="12"/>
+      <c r="BT26" s="12"/>
+      <c r="BU26" s="12"/>
+      <c r="BV26" s="12"/>
+      <c r="BW26" s="12"/>
+      <c r="BX26" s="12"/>
     </row>
     <row r="27" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>4</v>
-      </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
-      <c r="O27" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="14"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="14"/>
+      <c r="Q27" s="12"/>
+      <c r="R27" s="12"/>
+      <c r="S27" s="12"/>
+      <c r="T27" s="12"/>
+      <c r="U27" s="12"/>
+      <c r="V27" s="12"/>
+      <c r="W27" s="12"/>
+      <c r="X27" s="12"/>
+      <c r="Y27" s="12"/>
+      <c r="Z27" s="14"/>
+      <c r="AA27" s="12"/>
+      <c r="AB27" s="12"/>
+      <c r="AC27" s="12"/>
+      <c r="AD27" s="12"/>
+      <c r="AE27" s="13"/>
+      <c r="AF27" s="13"/>
+      <c r="AG27" s="13"/>
+      <c r="AH27" s="14"/>
+      <c r="AI27" s="15"/>
+      <c r="AJ27" s="14"/>
+      <c r="AK27" s="12"/>
+      <c r="AL27" s="12"/>
+      <c r="AM27" s="12"/>
+      <c r="AN27" s="12"/>
+      <c r="AO27" s="12"/>
+      <c r="AP27" s="14"/>
+      <c r="AQ27" s="13"/>
+      <c r="AR27" s="13"/>
+      <c r="AS27" s="13"/>
+      <c r="AT27" s="13"/>
+      <c r="AU27" s="13"/>
+      <c r="AV27" s="13"/>
+      <c r="AW27" s="13"/>
+      <c r="AX27" s="13"/>
+      <c r="AY27" s="13"/>
+      <c r="AZ27" s="13"/>
+      <c r="BA27" s="13"/>
+      <c r="BB27" s="13"/>
+      <c r="BC27" s="13"/>
+      <c r="BD27" s="14"/>
+      <c r="BE27" s="15"/>
+      <c r="BF27" s="14"/>
+      <c r="BG27" s="12"/>
+      <c r="BH27" s="12"/>
+      <c r="BI27" s="12"/>
+      <c r="BJ27" s="12"/>
+      <c r="BK27" s="12"/>
+      <c r="BL27" s="12"/>
+      <c r="BM27" s="12"/>
+      <c r="BN27" s="14"/>
+      <c r="BO27" s="15"/>
+      <c r="BP27" s="14"/>
+      <c r="BQ27" s="12"/>
+      <c r="BR27" s="12"/>
+      <c r="BS27" s="12"/>
+      <c r="BT27" s="12"/>
+      <c r="BU27" s="12"/>
+      <c r="BV27" s="12"/>
+      <c r="BW27" s="12"/>
+      <c r="BX27" s="12"/>
     </row>
     <row r="28" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>3</v>
-      </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
-      <c r="N28" s="1"/>
-      <c r="O28" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="12"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="12"/>
+      <c r="Q28" s="14"/>
+      <c r="R28" s="12"/>
+      <c r="S28" s="12"/>
+      <c r="T28" s="12"/>
+      <c r="U28" s="12"/>
+      <c r="V28" s="12"/>
+      <c r="W28" s="12"/>
+      <c r="X28" s="12"/>
+      <c r="Y28" s="14"/>
+      <c r="Z28" s="12"/>
+      <c r="AA28" s="12"/>
+      <c r="AB28" s="12"/>
+      <c r="AC28" s="12"/>
+      <c r="AD28" s="12"/>
+      <c r="AE28" s="12"/>
+      <c r="AF28" s="12"/>
+      <c r="AG28" s="12"/>
+      <c r="AH28" s="12"/>
+      <c r="AI28" s="12"/>
+      <c r="AJ28" s="12"/>
+      <c r="AK28" s="14"/>
+      <c r="AL28" s="12"/>
+      <c r="AM28" s="12"/>
+      <c r="AN28" s="12"/>
+      <c r="AO28" s="14"/>
+      <c r="AP28" s="12"/>
+      <c r="AQ28" s="12"/>
+      <c r="AR28" s="12"/>
+      <c r="AS28" s="12"/>
+      <c r="AT28" s="12"/>
+      <c r="AU28" s="12"/>
+      <c r="AV28" s="12"/>
+      <c r="AW28" s="12"/>
+      <c r="AX28" s="12"/>
+      <c r="AY28" s="12"/>
+      <c r="AZ28" s="12"/>
+      <c r="BA28" s="12"/>
+      <c r="BB28" s="12"/>
+      <c r="BC28" s="12"/>
+      <c r="BD28" s="12"/>
+      <c r="BE28" s="12"/>
+      <c r="BF28" s="12"/>
+      <c r="BG28" s="12"/>
+      <c r="BH28" s="12"/>
+      <c r="BI28" s="12"/>
+      <c r="BJ28" s="12"/>
+      <c r="BK28" s="12"/>
+      <c r="BL28" s="13"/>
+      <c r="BM28" s="13"/>
+      <c r="BN28" s="13"/>
+      <c r="BO28" s="13"/>
+      <c r="BP28" s="13"/>
+      <c r="BQ28" s="14"/>
+      <c r="BR28" s="15"/>
+      <c r="BS28" s="14"/>
+      <c r="BT28" s="12"/>
+      <c r="BU28" s="12"/>
+      <c r="BV28" s="12"/>
+      <c r="BW28" s="12"/>
+      <c r="BX28" s="12"/>
     </row>
     <row r="29" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>2</v>
-      </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="B29" s="12"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
+      <c r="N29" s="13"/>
+      <c r="O29" s="13"/>
+      <c r="P29" s="13"/>
+      <c r="Q29" s="13"/>
+      <c r="R29" s="14"/>
+      <c r="S29" s="15"/>
+      <c r="T29" s="14"/>
+      <c r="U29" s="12"/>
+      <c r="V29" s="12"/>
+      <c r="W29" s="12"/>
+      <c r="X29" s="14"/>
+      <c r="Y29" s="12"/>
+      <c r="Z29" s="12"/>
+      <c r="AA29" s="12"/>
+      <c r="AB29" s="12"/>
+      <c r="AC29" s="12"/>
+      <c r="AD29" s="12"/>
+      <c r="AE29" s="12"/>
+      <c r="AF29" s="12"/>
+      <c r="AG29" s="12"/>
+      <c r="AH29" s="13"/>
+      <c r="AI29" s="13"/>
+      <c r="AJ29" s="13"/>
+      <c r="AK29" s="13"/>
+      <c r="AL29" s="14"/>
+      <c r="AM29" s="15"/>
+      <c r="AN29" s="14"/>
+      <c r="AO29" s="12"/>
+      <c r="AP29" s="12"/>
+      <c r="AQ29" s="12"/>
+      <c r="AR29" s="12"/>
+      <c r="AS29" s="12"/>
+      <c r="AT29" s="12"/>
+      <c r="AU29" s="12"/>
+      <c r="AV29" s="12"/>
+      <c r="AW29" s="12"/>
+      <c r="AX29" s="12"/>
+      <c r="AY29" s="12"/>
+      <c r="AZ29" s="12"/>
+      <c r="BA29" s="12"/>
+      <c r="BB29" s="12"/>
+      <c r="BC29" s="12"/>
+      <c r="BD29" s="12"/>
+      <c r="BE29" s="12"/>
+      <c r="BF29" s="12"/>
+      <c r="BG29" s="12"/>
+      <c r="BH29" s="12"/>
+      <c r="BI29" s="12"/>
+      <c r="BJ29" s="12"/>
+      <c r="BK29" s="12"/>
+      <c r="BL29" s="12"/>
+      <c r="BM29" s="12"/>
+      <c r="BN29" s="12"/>
+      <c r="BO29" s="12"/>
+      <c r="BP29" s="12"/>
+      <c r="BQ29" s="12"/>
+      <c r="BR29" s="12"/>
+      <c r="BS29" s="12"/>
+      <c r="BT29" s="12"/>
+      <c r="BU29" s="12"/>
+      <c r="BV29" s="12"/>
+      <c r="BW29" s="12"/>
+      <c r="BX29" s="12"/>
     </row>
     <row r="30" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A30">
+        <v>0</v>
+      </c>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="12"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="12"/>
+      <c r="P30" s="12"/>
+      <c r="Q30" s="12"/>
+      <c r="R30" s="13"/>
+      <c r="S30" s="13"/>
+      <c r="T30" s="13"/>
+      <c r="U30" s="14"/>
+      <c r="V30" s="15"/>
+      <c r="W30" s="14"/>
+      <c r="X30" s="12"/>
+      <c r="Y30" s="12"/>
+      <c r="Z30" s="12"/>
+      <c r="AA30" s="12"/>
+      <c r="AB30" s="12"/>
+      <c r="AC30" s="12"/>
+      <c r="AD30" s="12"/>
+      <c r="AE30" s="12"/>
+      <c r="AF30" s="12"/>
+      <c r="AG30" s="12"/>
+      <c r="AH30" s="12"/>
+      <c r="AI30" s="12"/>
+      <c r="AJ30" s="12"/>
+      <c r="AK30" s="12"/>
+      <c r="AL30" s="12"/>
+      <c r="AM30" s="12"/>
+      <c r="AN30" s="12"/>
+      <c r="AO30" s="12"/>
+      <c r="AP30" s="12"/>
+      <c r="AQ30" s="12"/>
+      <c r="AR30" s="12"/>
+      <c r="AS30" s="12"/>
+      <c r="AT30" s="12"/>
+      <c r="AU30" s="12"/>
+      <c r="AV30" s="12"/>
+      <c r="AW30" s="12"/>
+      <c r="AX30" s="12"/>
+      <c r="AY30" s="12"/>
+      <c r="AZ30" s="12"/>
+      <c r="BA30" s="12"/>
+      <c r="BB30" s="12"/>
+      <c r="BC30" s="12"/>
+      <c r="BD30" s="12"/>
+      <c r="BE30" s="12"/>
+      <c r="BF30" s="12"/>
+      <c r="BG30" s="12"/>
+      <c r="BH30" s="12"/>
+      <c r="BI30" s="12"/>
+      <c r="BJ30" s="12"/>
+      <c r="BK30" s="12"/>
+      <c r="BL30" s="12"/>
+      <c r="BM30" s="12"/>
+      <c r="BN30" s="12"/>
+      <c r="BO30" s="12"/>
+      <c r="BP30" s="12"/>
+      <c r="BQ30" s="12"/>
+      <c r="BR30" s="12"/>
+      <c r="BS30" s="12"/>
+      <c r="BT30" s="12"/>
+      <c r="BU30" s="12"/>
+      <c r="BV30" s="12"/>
+      <c r="BW30" s="12"/>
+      <c r="BX30" s="12"/>
+    </row>
+    <row r="31" spans="1:76" x14ac:dyDescent="0.25">
+      <c r="D31"/>
+    </row>
+    <row r="32" spans="1:76" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
         <v>1</v>
       </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
-      <c r="O30" s="1"/>
-    </row>
-    <row r="31" spans="1:76" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>0</v>
-      </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
-      <c r="N31" s="1"/>
-      <c r="O31" s="1"/>
-    </row>
-    <row r="32" spans="1:76" x14ac:dyDescent="0.25">
-      <c r="P32" s="4"/>
-      <c r="Q32" s="4"/>
-      <c r="R32" s="4"/>
-      <c r="S32" s="4"/>
-      <c r="T32" s="4"/>
-      <c r="U32" s="4"/>
-      <c r="V32" s="4"/>
-      <c r="W32" s="4"/>
-      <c r="X32" s="4"/>
-      <c r="Y32" s="4"/>
-      <c r="Z32" s="4"/>
-      <c r="AA32" s="4"/>
-      <c r="AB32" s="4"/>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="E32">
+        <v>3</v>
+      </c>
+      <c r="F32">
+        <v>4</v>
+      </c>
+      <c r="G32">
+        <v>5</v>
+      </c>
+      <c r="H32">
+        <v>6</v>
+      </c>
+      <c r="I32">
+        <v>7</v>
+      </c>
+      <c r="J32">
+        <v>8</v>
+      </c>
+      <c r="K32">
+        <v>9</v>
+      </c>
+      <c r="L32">
+        <v>10</v>
+      </c>
+      <c r="M32">
+        <v>11</v>
+      </c>
+      <c r="N32">
+        <v>12</v>
+      </c>
     </row>
     <row r="33" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>4</v>
-      </c>
-      <c r="B33">
-        <v>0</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
-      </c>
-      <c r="D33">
-        <v>2</v>
-      </c>
-      <c r="E33">
-        <v>3</v>
-      </c>
-      <c r="F33">
-        <v>4</v>
-      </c>
-      <c r="G33">
-        <v>5</v>
-      </c>
-      <c r="H33">
-        <v>6</v>
-      </c>
-      <c r="I33">
-        <v>7</v>
-      </c>
-      <c r="J33">
+      <c r="A33">
         <v>8</v>
       </c>
-      <c r="K33">
-        <v>9</v>
-      </c>
-      <c r="L33">
-        <v>10</v>
-      </c>
-      <c r="M33">
-        <v>11</v>
-      </c>
-      <c r="N33">
-        <v>12</v>
-      </c>
-      <c r="P33" s="4"/>
-      <c r="Q33" s="4"/>
-      <c r="R33" s="4"/>
-      <c r="S33" s="4"/>
-      <c r="T33" s="4"/>
-      <c r="U33" s="4"/>
-      <c r="V33" s="4"/>
-      <c r="W33" s="4"/>
-      <c r="X33" s="4"/>
-      <c r="Y33" s="4"/>
-      <c r="Z33" s="4"/>
-      <c r="AA33" s="4"/>
-      <c r="AB33" s="4"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
     </row>
     <row r="34" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -2872,23 +3675,10 @@
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
-      <c r="P34" s="4"/>
-      <c r="Q34" s="4"/>
-      <c r="R34" s="4"/>
-      <c r="S34" s="4"/>
-      <c r="T34" s="4"/>
-      <c r="U34" s="4"/>
-      <c r="V34" s="4"/>
-      <c r="W34" s="4"/>
-      <c r="X34" s="4"/>
-      <c r="Y34" s="4"/>
-      <c r="Z34" s="4"/>
-      <c r="AA34" s="4"/>
-      <c r="AB34" s="4"/>
     </row>
     <row r="35" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -2904,30 +3694,17 @@
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
-      <c r="P35" s="4"/>
-      <c r="Q35" s="4"/>
-      <c r="R35" s="4"/>
-      <c r="S35" s="4"/>
-      <c r="T35" s="4"/>
-      <c r="U35" s="4"/>
-      <c r="V35" s="4"/>
-      <c r="W35" s="4"/>
-      <c r="X35" s="4"/>
-      <c r="Y35" s="4"/>
-      <c r="Z35" s="4"/>
-      <c r="AA35" s="4"/>
-      <c r="AB35" s="4"/>
     </row>
     <row r="36" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="2"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
@@ -2936,31 +3713,18 @@
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
-      <c r="P36" s="4"/>
-      <c r="Q36" s="4"/>
-      <c r="R36" s="4"/>
-      <c r="S36" s="4"/>
-      <c r="T36" s="4"/>
-      <c r="U36" s="4"/>
-      <c r="V36" s="4"/>
-      <c r="W36" s="4"/>
-      <c r="X36" s="4"/>
-      <c r="Y36" s="4"/>
-      <c r="Z36" s="4"/>
-      <c r="AA36" s="4"/>
-      <c r="AB36" s="4"/>
     </row>
     <row r="37" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
+      <c r="F37" s="2"/>
       <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
+      <c r="H37" s="2"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
@@ -2968,125 +3732,73 @@
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
-      <c r="P37" s="4"/>
-      <c r="Q37" s="4"/>
-      <c r="R37" s="4"/>
-      <c r="S37" s="4"/>
-      <c r="T37" s="4"/>
-      <c r="U37" s="4"/>
-      <c r="V37" s="4"/>
-      <c r="W37" s="4"/>
-      <c r="X37" s="4"/>
-      <c r="Y37" s="4"/>
-      <c r="Z37" s="4"/>
-      <c r="AA37" s="4"/>
-      <c r="AB37" s="4"/>
     </row>
     <row r="38" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>4</v>
-      </c>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
+        <v>3</v>
+      </c>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
+      <c r="I38" s="2"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
-      <c r="P38" s="4"/>
-      <c r="Q38" s="4"/>
-      <c r="R38" s="4"/>
-      <c r="S38" s="4"/>
-      <c r="T38" s="4"/>
-      <c r="U38" s="4"/>
-      <c r="V38" s="4"/>
-      <c r="W38" s="4"/>
-      <c r="X38" s="4"/>
-      <c r="Y38" s="4"/>
-      <c r="Z38" s="4"/>
-      <c r="AA38" s="4"/>
-      <c r="AB38" s="4"/>
     </row>
     <row r="39" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="2"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
-      <c r="P39" s="4"/>
-      <c r="Q39" s="4"/>
-      <c r="R39" s="4"/>
-      <c r="S39" s="4"/>
-      <c r="T39" s="4"/>
-      <c r="U39" s="4"/>
-      <c r="V39" s="4"/>
-      <c r="W39" s="4"/>
-      <c r="X39" s="4"/>
-      <c r="Y39" s="4"/>
-      <c r="Z39" s="4"/>
-      <c r="AA39" s="4"/>
-      <c r="AB39" s="4"/>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>2</v>
-      </c>
-      <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="B40" s="1"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
+      <c r="K40" s="2"/>
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
-      <c r="P40" s="4"/>
-      <c r="Q40" s="4"/>
-      <c r="R40" s="4"/>
-      <c r="S40" s="4"/>
-      <c r="T40" s="4"/>
-      <c r="U40" s="4"/>
-      <c r="V40" s="4"/>
-      <c r="W40" s="4"/>
-      <c r="X40" s="4"/>
-      <c r="Y40" s="4"/>
-      <c r="Z40" s="4"/>
-      <c r="AA40" s="4"/>
-      <c r="AB40" s="4"/>
     </row>
     <row r="41" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>1</v>
-      </c>
-      <c r="B41" s="1"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
+        <v>0</v>
+      </c>
+      <c r="B41" s="2"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
@@ -3096,38 +3808,8 @@
       <c r="M41" s="1"/>
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
-      <c r="P41" s="4"/>
-      <c r="Q41" s="4"/>
-      <c r="R41" s="4"/>
-      <c r="S41" s="4"/>
-      <c r="T41" s="4"/>
-      <c r="U41" s="4"/>
-      <c r="V41" s="4"/>
-      <c r="W41" s="4"/>
-      <c r="X41" s="4"/>
-      <c r="Y41" s="4"/>
-      <c r="Z41" s="4"/>
-      <c r="AA41" s="4"/>
-      <c r="AB41" s="4"/>
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>0</v>
-      </c>
-      <c r="B42" s="2"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
-      <c r="L42" s="1"/>
-      <c r="M42" s="1"/>
-      <c r="N42" s="1"/>
-      <c r="O42" s="1"/>
       <c r="P42" s="4"/>
       <c r="Q42" s="4"/>
       <c r="R42" s="4"/>
@@ -3143,20 +3825,48 @@
       <c r="AB42" s="4"/>
     </row>
     <row r="43" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B43" s="2"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
-      <c r="K43" s="1"/>
-      <c r="L43" s="1"/>
-      <c r="M43" s="1"/>
-      <c r="N43" s="1"/>
-      <c r="O43" s="1"/>
+      <c r="A43" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
+      <c r="E43">
+        <v>3</v>
+      </c>
+      <c r="F43">
+        <v>4</v>
+      </c>
+      <c r="G43">
+        <v>5</v>
+      </c>
+      <c r="H43">
+        <v>6</v>
+      </c>
+      <c r="I43">
+        <v>7</v>
+      </c>
+      <c r="J43">
+        <v>8</v>
+      </c>
+      <c r="K43">
+        <v>9</v>
+      </c>
+      <c r="L43">
+        <v>10</v>
+      </c>
+      <c r="M43">
+        <v>11</v>
+      </c>
+      <c r="N43">
+        <v>12</v>
+      </c>
       <c r="P43" s="4"/>
       <c r="Q43" s="4"/>
       <c r="R43" s="4"/>
@@ -3172,7 +3882,10 @@
       <c r="AB43" s="4"/>
     </row>
     <row r="44" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B44" s="2"/>
+      <c r="A44">
+        <v>8</v>
+      </c>
+      <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
@@ -3186,54 +3899,55 @@
       <c r="M44" s="1"/>
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
+      <c r="P44" s="4"/>
+      <c r="Q44" s="4"/>
+      <c r="R44" s="4"/>
+      <c r="S44" s="4"/>
+      <c r="T44" s="4"/>
+      <c r="U44" s="4"/>
+      <c r="V44" s="4"/>
+      <c r="W44" s="4"/>
+      <c r="X44" s="4"/>
+      <c r="Y44" s="4"/>
+      <c r="Z44" s="4"/>
+      <c r="AA44" s="4"/>
+      <c r="AB44" s="4"/>
     </row>
     <row r="45" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>6</v>
-      </c>
-      <c r="B45" s="11">
-        <v>0</v>
-      </c>
-      <c r="C45" s="11">
-        <v>1</v>
-      </c>
-      <c r="D45" s="11">
-        <v>2</v>
-      </c>
-      <c r="E45" s="11">
-        <v>3</v>
-      </c>
-      <c r="F45" s="11">
-        <v>4</v>
-      </c>
-      <c r="G45" s="11">
-        <v>5</v>
-      </c>
-      <c r="H45" s="11">
-        <v>6</v>
-      </c>
-      <c r="I45" s="11">
+      <c r="A45">
         <v>7</v>
       </c>
-      <c r="J45" s="11">
-        <v>8</v>
-      </c>
-      <c r="K45" s="11">
-        <v>9</v>
-      </c>
-      <c r="L45" s="11">
-        <v>10</v>
-      </c>
-      <c r="M45" s="11">
-        <v>11</v>
-      </c>
-      <c r="N45" s="11">
-        <v>12</v>
-      </c>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+      <c r="L45" s="1"/>
+      <c r="M45" s="1"/>
+      <c r="N45" s="1"/>
+      <c r="O45" s="1"/>
+      <c r="P45" s="4"/>
+      <c r="Q45" s="4"/>
+      <c r="R45" s="4"/>
+      <c r="S45" s="4"/>
+      <c r="T45" s="4"/>
+      <c r="U45" s="4"/>
+      <c r="V45" s="4"/>
+      <c r="W45" s="4"/>
+      <c r="X45" s="4"/>
+      <c r="Y45" s="4"/>
+      <c r="Z45" s="4"/>
+      <c r="AA45" s="4"/>
+      <c r="AB45" s="4"/>
     </row>
     <row r="46" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -3249,10 +3963,23 @@
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
+      <c r="P46" s="4"/>
+      <c r="Q46" s="4"/>
+      <c r="R46" s="4"/>
+      <c r="S46" s="4"/>
+      <c r="T46" s="4"/>
+      <c r="U46" s="4"/>
+      <c r="V46" s="4"/>
+      <c r="W46" s="4"/>
+      <c r="X46" s="4"/>
+      <c r="Y46" s="4"/>
+      <c r="Z46" s="4"/>
+      <c r="AA46" s="4"/>
+      <c r="AB46" s="4"/>
     </row>
     <row r="47" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -3268,16 +3995,29 @@
       <c r="M47" s="1"/>
       <c r="N47" s="1"/>
       <c r="O47" s="1"/>
+      <c r="P47" s="4"/>
+      <c r="Q47" s="4"/>
+      <c r="R47" s="4"/>
+      <c r="S47" s="4"/>
+      <c r="T47" s="4"/>
+      <c r="U47" s="4"/>
+      <c r="V47" s="4"/>
+      <c r="W47" s="4"/>
+      <c r="X47" s="4"/>
+      <c r="Y47" s="4"/>
+      <c r="Z47" s="4"/>
+      <c r="AA47" s="4"/>
+      <c r="AB47" s="4"/>
     </row>
     <row r="48" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
@@ -3287,10 +4027,23 @@
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P48" s="4"/>
+      <c r="Q48" s="4"/>
+      <c r="R48" s="4"/>
+      <c r="S48" s="4"/>
+      <c r="T48" s="4"/>
+      <c r="U48" s="4"/>
+      <c r="V48" s="4"/>
+      <c r="W48" s="4"/>
+      <c r="X48" s="4"/>
+      <c r="Y48" s="4"/>
+      <c r="Z48" s="4"/>
+      <c r="AA48" s="4"/>
+      <c r="AB48" s="4"/>
+    </row>
+    <row r="49" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -3306,16 +4059,29 @@
       <c r="M49" s="1"/>
       <c r="N49" s="1"/>
       <c r="O49" s="1"/>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P49" s="4"/>
+      <c r="Q49" s="4"/>
+      <c r="R49" s="4"/>
+      <c r="S49" s="4"/>
+      <c r="T49" s="4"/>
+      <c r="U49" s="4"/>
+      <c r="V49" s="4"/>
+      <c r="W49" s="4"/>
+      <c r="X49" s="4"/>
+      <c r="Y49" s="4"/>
+      <c r="Z49" s="4"/>
+      <c r="AA49" s="4"/>
+      <c r="AB49" s="4"/>
+    </row>
+    <row r="50" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>4</v>
-      </c>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="2"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
@@ -3325,51 +4091,87 @@
       <c r="M50" s="1"/>
       <c r="N50" s="1"/>
       <c r="O50" s="1"/>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P50" s="4"/>
+      <c r="Q50" s="4"/>
+      <c r="R50" s="4"/>
+      <c r="S50" s="4"/>
+      <c r="T50" s="4"/>
+      <c r="U50" s="4"/>
+      <c r="V50" s="4"/>
+      <c r="W50" s="4"/>
+      <c r="X50" s="4"/>
+      <c r="Y50" s="4"/>
+      <c r="Z50" s="4"/>
+      <c r="AA50" s="4"/>
+      <c r="AB50" s="4"/>
+    </row>
+    <row r="51" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>3</v>
-      </c>
-      <c r="B51" s="9"/>
-      <c r="C51" s="9"/>
+        <v>1</v>
+      </c>
+      <c r="B51" s="1"/>
+      <c r="C51" s="2"/>
       <c r="D51" s="9"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="10"/>
-      <c r="G51" s="2"/>
-      <c r="H51" s="9"/>
-      <c r="I51" s="9"/>
-      <c r="J51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
       <c r="N51" s="1"/>
       <c r="O51" s="1"/>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P51" s="4"/>
+      <c r="Q51" s="4"/>
+      <c r="R51" s="4"/>
+      <c r="S51" s="4"/>
+      <c r="T51" s="4"/>
+      <c r="U51" s="4"/>
+      <c r="V51" s="4"/>
+      <c r="W51" s="4"/>
+      <c r="X51" s="4"/>
+      <c r="Y51" s="4"/>
+      <c r="Z51" s="4"/>
+      <c r="AA51" s="4"/>
+      <c r="AB51" s="4"/>
+    </row>
+    <row r="52" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>2</v>
-      </c>
-      <c r="B52" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="B52" s="2"/>
       <c r="C52" s="1"/>
-      <c r="D52" s="2"/>
+      <c r="D52" s="1"/>
       <c r="E52" s="1"/>
-      <c r="F52" s="9"/>
-      <c r="G52" s="9"/>
-      <c r="H52" s="2"/>
-      <c r="I52" s="10"/>
-      <c r="J52" s="2"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
       <c r="K52" s="1"/>
       <c r="L52" s="1"/>
       <c r="M52" s="1"/>
       <c r="N52" s="1"/>
       <c r="O52" s="1"/>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>1</v>
-      </c>
-      <c r="B53" s="1"/>
-      <c r="C53" s="2"/>
+      <c r="P52" s="4"/>
+      <c r="Q52" s="4"/>
+      <c r="R52" s="4"/>
+      <c r="S52" s="4"/>
+      <c r="T52" s="4"/>
+      <c r="U52" s="4"/>
+      <c r="V52" s="4"/>
+      <c r="W52" s="4"/>
+      <c r="X52" s="4"/>
+      <c r="Y52" s="4"/>
+      <c r="Z52" s="4"/>
+      <c r="AA52" s="4"/>
+      <c r="AB52" s="4"/>
+    </row>
+    <row r="53" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B53" s="2"/>
+      <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
@@ -3377,83 +4179,110 @@
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
-      <c r="K53" s="2"/>
+      <c r="K53" s="1"/>
       <c r="L53" s="1"/>
       <c r="M53" s="1"/>
       <c r="N53" s="1"/>
       <c r="O53" s="1"/>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>0</v>
-      </c>
+      <c r="P53" s="4"/>
+      <c r="Q53" s="4"/>
+      <c r="R53" s="4"/>
+      <c r="S53" s="4"/>
+      <c r="T53" s="4"/>
+      <c r="U53" s="4"/>
+      <c r="V53" s="4"/>
+      <c r="W53" s="4"/>
+      <c r="X53" s="4"/>
+      <c r="Y53" s="4"/>
+      <c r="Z53" s="4"/>
+      <c r="AA53" s="4"/>
+      <c r="AB53" s="4"/>
+    </row>
+    <row r="54" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B54" s="2"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
-      <c r="H54" s="9"/>
-      <c r="I54" s="9"/>
-      <c r="J54" s="9"/>
-      <c r="K54" s="9"/>
-      <c r="L54" s="2"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
+      <c r="L54" s="1"/>
       <c r="M54" s="1"/>
       <c r="N54" s="1"/>
       <c r="O54" s="1"/>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="55" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>6</v>
+      </c>
+      <c r="B55" s="11">
+        <v>0</v>
+      </c>
+      <c r="C55" s="11">
+        <v>1</v>
+      </c>
+      <c r="D55" s="11">
+        <v>2</v>
+      </c>
+      <c r="E55" s="11">
+        <v>3</v>
+      </c>
+      <c r="F55" s="11">
+        <v>4</v>
+      </c>
+      <c r="G55" s="11">
         <v>5</v>
       </c>
-      <c r="B56">
-        <v>0</v>
-      </c>
-      <c r="C56">
-        <v>1</v>
-      </c>
-      <c r="D56">
-        <v>5</v>
-      </c>
-      <c r="E56">
+      <c r="H55" s="11">
         <v>6</v>
       </c>
-      <c r="F56">
+      <c r="I55" s="11">
         <v>7</v>
       </c>
-      <c r="G56">
+      <c r="J55" s="11">
         <v>8</v>
       </c>
-      <c r="H56">
+      <c r="K55" s="11">
         <v>9</v>
       </c>
-      <c r="I56">
+      <c r="L55" s="11">
         <v>10</v>
       </c>
-      <c r="J56">
+      <c r="M55" s="11">
         <v>11</v>
       </c>
-      <c r="K56">
+      <c r="N55" s="11">
         <v>12</v>
       </c>
-      <c r="L56">
-        <v>13</v>
-      </c>
-      <c r="M56">
-        <v>14</v>
-      </c>
-      <c r="N56">
-        <v>15</v>
-      </c>
-      <c r="O56">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>8</v>
+      </c>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+      <c r="K56" s="1"/>
+      <c r="L56" s="1"/>
+      <c r="M56" s="1"/>
+      <c r="N56" s="1"/>
+      <c r="O56" s="1"/>
+    </row>
+    <row r="57" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
@@ -3467,11 +4296,12 @@
       <c r="N57" s="1"/>
       <c r="O57" s="1"/>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
@@ -3485,30 +4315,32 @@
       <c r="N58" s="1"/>
       <c r="O58" s="1"/>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
       <c r="D59" s="1"/>
-      <c r="E59" s="3"/>
-      <c r="F59" s="3"/>
-      <c r="G59" s="3"/>
-      <c r="H59" s="3"/>
-      <c r="I59" s="3"/>
-      <c r="J59" s="3"/>
-      <c r="K59" s="3"/>
-      <c r="L59" s="3"/>
-      <c r="M59" s="2"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+      <c r="K59" s="1"/>
+      <c r="L59" s="1"/>
+      <c r="M59" s="1"/>
       <c r="N59" s="1"/>
       <c r="O59" s="1"/>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>5</v>
-      </c>
-      <c r="B60" s="3"/>
-      <c r="D60" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
@@ -3516,40 +4348,42 @@
       <c r="I60" s="1"/>
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
-      <c r="L60" s="2"/>
+      <c r="L60" s="1"/>
       <c r="M60" s="1"/>
       <c r="N60" s="1"/>
       <c r="O60" s="1"/>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>4</v>
-      </c>
-      <c r="B61" s="1"/>
-      <c r="D61" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="B61" s="9"/>
+      <c r="C61" s="9"/>
+      <c r="D61" s="9"/>
       <c r="E61" s="2"/>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
-      <c r="H61" s="1"/>
-      <c r="I61" s="1"/>
-      <c r="J61" s="1"/>
-      <c r="K61" s="2"/>
+      <c r="F61" s="10"/>
+      <c r="G61" s="2"/>
+      <c r="H61" s="9"/>
+      <c r="I61" s="9"/>
+      <c r="J61" s="9"/>
+      <c r="K61" s="1"/>
       <c r="L61" s="1"/>
       <c r="M61" s="1"/>
       <c r="N61" s="1"/>
       <c r="O61" s="1"/>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B62" s="1"/>
-      <c r="D62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="2"/>
       <c r="E62" s="1"/>
-      <c r="F62" s="2"/>
-      <c r="G62" s="1"/>
-      <c r="H62" s="1"/>
-      <c r="I62" s="1"/>
+      <c r="F62" s="9"/>
+      <c r="G62" s="9"/>
+      <c r="H62" s="2"/>
+      <c r="I62" s="10"/>
       <c r="J62" s="2"/>
       <c r="K62" s="1"/>
       <c r="L62" s="1"/>
@@ -3557,90 +4391,150 @@
       <c r="N62" s="1"/>
       <c r="O62" s="1"/>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B63" s="1"/>
+      <c r="C63" s="2"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
-      <c r="G63" s="2"/>
+      <c r="G63" s="1"/>
       <c r="H63" s="1"/>
-      <c r="I63" s="2"/>
+      <c r="I63" s="1"/>
       <c r="J63" s="1"/>
-      <c r="K63" s="1"/>
+      <c r="K63" s="2"/>
       <c r="L63" s="1"/>
       <c r="M63" s="1"/>
       <c r="N63" s="1"/>
       <c r="O63" s="1"/>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>1</v>
-      </c>
-      <c r="B64" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="B64" s="2"/>
+      <c r="C64" s="1"/>
       <c r="D64" s="1"/>
-      <c r="E64" s="3"/>
-      <c r="F64" s="3"/>
-      <c r="G64" s="3"/>
-      <c r="H64" s="2"/>
-      <c r="I64" s="1"/>
-      <c r="J64" s="1"/>
-      <c r="K64" s="1"/>
-      <c r="L64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+      <c r="H64" s="9"/>
+      <c r="I64" s="9"/>
+      <c r="J64" s="9"/>
+      <c r="K64" s="9"/>
+      <c r="L64" s="2"/>
       <c r="M64" s="1"/>
       <c r="N64" s="1"/>
       <c r="O64" s="1"/>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A65">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>5</v>
+      </c>
+      <c r="B66">
         <v>0</v>
       </c>
-      <c r="B65" s="2"/>
-      <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
-      <c r="G65" s="1"/>
-      <c r="H65" s="1"/>
-      <c r="I65" s="1"/>
-      <c r="J65" s="1"/>
-      <c r="K65" s="1"/>
-      <c r="L65" s="1"/>
-      <c r="M65" s="1"/>
-      <c r="N65" s="1"/>
-      <c r="O65" s="1"/>
+      <c r="C66">
+        <v>1</v>
+      </c>
+      <c r="D66">
+        <v>5</v>
+      </c>
+      <c r="E66">
+        <v>6</v>
+      </c>
+      <c r="F66">
+        <v>7</v>
+      </c>
+      <c r="G66">
+        <v>8</v>
+      </c>
+      <c r="H66">
+        <v>9</v>
+      </c>
+      <c r="I66">
+        <v>10</v>
+      </c>
+      <c r="J66">
+        <v>11</v>
+      </c>
+      <c r="K66">
+        <v>12</v>
+      </c>
+      <c r="L66">
+        <v>13</v>
+      </c>
+      <c r="M66">
+        <v>14</v>
+      </c>
+      <c r="N66">
+        <v>15</v>
+      </c>
+      <c r="O66">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>8</v>
+      </c>
+      <c r="B67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+      <c r="J67" s="1"/>
+      <c r="K67" s="1"/>
+      <c r="L67" s="1"/>
+      <c r="M67" s="1"/>
+      <c r="N67" s="1"/>
+      <c r="O67" s="1"/>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>1</v>
-      </c>
+      <c r="A68">
+        <v>7</v>
+      </c>
+      <c r="B68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
+      <c r="J68" s="1"/>
+      <c r="K68" s="1"/>
+      <c r="L68" s="1"/>
+      <c r="M68" s="1"/>
+      <c r="N68" s="1"/>
+      <c r="O68" s="1"/>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>4</v>
-      </c>
-      <c r="B69" s="3"/>
-      <c r="C69" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="B69" s="1"/>
       <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
-      <c r="H69" s="1"/>
-      <c r="I69" s="1"/>
-      <c r="J69" s="1"/>
-      <c r="K69" s="1"/>
-      <c r="L69" s="1"/>
-      <c r="M69" s="1"/>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3"/>
+      <c r="G69" s="3"/>
+      <c r="H69" s="3"/>
+      <c r="I69" s="3"/>
+      <c r="J69" s="3"/>
+      <c r="K69" s="3"/>
+      <c r="L69" s="3"/>
+      <c r="M69" s="2"/>
       <c r="N69" s="1"/>
       <c r="O69" s="1"/>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>3</v>
-      </c>
-      <c r="B70" s="2"/>
-      <c r="C70" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="B70" s="3"/>
       <c r="D70" s="2"/>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
@@ -3649,17 +4543,16 @@
       <c r="I70" s="1"/>
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
-      <c r="L70" s="1"/>
+      <c r="L70" s="2"/>
       <c r="M70" s="1"/>
       <c r="N70" s="1"/>
       <c r="O70" s="1"/>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>2</v>
-      </c>
-      <c r="B71" s="3"/>
-      <c r="C71" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="B71" s="1"/>
       <c r="D71" s="3"/>
       <c r="E71" s="2"/>
       <c r="F71" s="1"/>
@@ -3667,7 +4560,7 @@
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
       <c r="J71" s="1"/>
-      <c r="K71" s="1"/>
+      <c r="K71" s="2"/>
       <c r="L71" s="1"/>
       <c r="M71" s="1"/>
       <c r="N71" s="1"/>
@@ -3675,17 +4568,16 @@
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
-      <c r="F72" s="1"/>
+      <c r="F72" s="2"/>
       <c r="G72" s="1"/>
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
-      <c r="J72" s="1"/>
+      <c r="J72" s="2"/>
       <c r="K72" s="1"/>
       <c r="L72" s="1"/>
       <c r="M72" s="1"/>
@@ -3694,16 +4586,15 @@
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B73" s="1"/>
-      <c r="C73" s="1"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
-      <c r="G73" s="1"/>
+      <c r="G73" s="2"/>
       <c r="H73" s="1"/>
-      <c r="I73" s="1"/>
+      <c r="I73" s="2"/>
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
       <c r="L73" s="1"/>
@@ -3711,42 +4602,59 @@
       <c r="N73" s="1"/>
       <c r="O73" s="1"/>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>1</v>
+      </c>
+      <c r="B74" s="1"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3"/>
+      <c r="G74" s="3"/>
+      <c r="H74" s="2"/>
+      <c r="I74" s="1"/>
+      <c r="J74" s="1"/>
+      <c r="K74" s="1"/>
+      <c r="L74" s="1"/>
+      <c r="M74" s="1"/>
+      <c r="N74" s="1"/>
+      <c r="O74" s="1"/>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A75">
         <v>0</v>
       </c>
+      <c r="B75" s="2"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+      <c r="H75" s="1"/>
+      <c r="I75" s="1"/>
+      <c r="J75" s="1"/>
+      <c r="K75" s="1"/>
+      <c r="L75" s="1"/>
+      <c r="M75" s="1"/>
+      <c r="N75" s="1"/>
+      <c r="O75" s="1"/>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A78">
-        <v>4</v>
-      </c>
-      <c r="B78" s="3"/>
-      <c r="C78" s="3"/>
-      <c r="D78" s="3"/>
-      <c r="E78" s="3"/>
-      <c r="F78" s="2"/>
-      <c r="G78" s="5"/>
-      <c r="H78" s="2"/>
-      <c r="I78" s="1"/>
-      <c r="J78" s="1"/>
-      <c r="K78" s="1"/>
-      <c r="L78" s="1"/>
-      <c r="M78" s="1"/>
-      <c r="N78" s="1"/>
-      <c r="O78" s="1"/>
+      <c r="A78" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>3</v>
-      </c>
-      <c r="B79" s="1"/>
-      <c r="C79" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="B79" s="3"/>
+      <c r="C79" s="2"/>
       <c r="D79" s="1"/>
-      <c r="E79" s="2"/>
+      <c r="E79" s="1"/>
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
       <c r="H79" s="1"/>
-      <c r="I79" s="2"/>
+      <c r="I79" s="1"/>
       <c r="J79" s="1"/>
       <c r="K79" s="1"/>
       <c r="L79" s="1"/>
@@ -3756,17 +4664,17 @@
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>2</v>
-      </c>
-      <c r="B80" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="B80" s="2"/>
       <c r="C80" s="1"/>
       <c r="D80" s="2"/>
-      <c r="E80" s="3"/>
-      <c r="F80" s="3"/>
-      <c r="G80" s="3"/>
-      <c r="H80" s="3"/>
-      <c r="I80" s="3"/>
-      <c r="J80" s="2"/>
+      <c r="E80" s="1"/>
+      <c r="F80" s="1"/>
+      <c r="G80" s="1"/>
+      <c r="H80" s="1"/>
+      <c r="I80" s="1"/>
+      <c r="J80" s="1"/>
       <c r="K80" s="1"/>
       <c r="L80" s="1"/>
       <c r="M80" s="1"/>
@@ -3775,12 +4683,12 @@
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>1</v>
-      </c>
-      <c r="B81" s="1"/>
-      <c r="C81" s="2"/>
-      <c r="D81" s="1"/>
-      <c r="E81" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="B81" s="3"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
+      <c r="E81" s="2"/>
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
       <c r="H81" s="1"/>
@@ -3794,9 +4702,9 @@
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>0</v>
-      </c>
-      <c r="B82" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
@@ -3811,76 +4719,48 @@
       <c r="N82" s="1"/>
       <c r="O82" s="1"/>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>3</v>
-      </c>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>0</v>
+      </c>
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1"/>
+      <c r="F83" s="1"/>
+      <c r="G83" s="1"/>
+      <c r="H83" s="1"/>
+      <c r="I83" s="1"/>
+      <c r="J83" s="1"/>
+      <c r="K83" s="1"/>
+      <c r="L83" s="1"/>
+      <c r="M83" s="1"/>
+      <c r="N83" s="1"/>
+      <c r="O83" s="1"/>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B86">
+      <c r="A86" t="s">
         <v>0</v>
       </c>
-      <c r="C86">
-        <v>1</v>
-      </c>
-      <c r="D86">
-        <v>2</v>
-      </c>
-      <c r="E86">
-        <v>3</v>
-      </c>
-      <c r="F86">
-        <v>4</v>
-      </c>
-      <c r="G86">
-        <v>5</v>
-      </c>
-      <c r="H86">
-        <v>6</v>
-      </c>
-      <c r="I86">
-        <v>7</v>
-      </c>
-      <c r="J86">
-        <v>8</v>
-      </c>
-      <c r="M86">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A87">
-        <v>5</v>
-      </c>
-      <c r="B87" s="3"/>
-      <c r="C87" s="3"/>
-      <c r="D87" s="3"/>
-      <c r="E87" s="3"/>
-      <c r="F87" s="3"/>
-      <c r="G87" s="2"/>
-      <c r="H87" s="1"/>
-      <c r="I87" s="1"/>
-      <c r="J87" s="1"/>
-      <c r="L87" s="1"/>
-      <c r="M87" s="1"/>
-      <c r="N87" s="1"/>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>4</v>
       </c>
-      <c r="B88" s="1"/>
-      <c r="C88" s="1"/>
-      <c r="D88" s="1"/>
-      <c r="E88" s="1"/>
+      <c r="B88" s="3"/>
+      <c r="C88" s="3"/>
+      <c r="D88" s="3"/>
+      <c r="E88" s="3"/>
       <c r="F88" s="2"/>
-      <c r="G88" s="1"/>
+      <c r="G88" s="5"/>
       <c r="H88" s="2"/>
       <c r="I88" s="1"/>
       <c r="J88" s="1"/>
+      <c r="K88" s="1"/>
       <c r="L88" s="1"/>
       <c r="M88" s="1"/>
       <c r="N88" s="1"/>
+      <c r="O88" s="1"/>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89">
@@ -3888,16 +4768,18 @@
       </c>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
-      <c r="D89" s="3"/>
+      <c r="D89" s="1"/>
       <c r="E89" s="2"/>
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
       <c r="H89" s="1"/>
       <c r="I89" s="2"/>
       <c r="J89" s="1"/>
+      <c r="K89" s="1"/>
       <c r="L89" s="1"/>
-      <c r="M89" s="3"/>
-      <c r="N89" s="2"/>
+      <c r="M89" s="1"/>
+      <c r="N89" s="1"/>
+      <c r="O89" s="1"/>
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90">
@@ -3912,9 +4794,11 @@
       <c r="H90" s="3"/>
       <c r="I90" s="3"/>
       <c r="J90" s="2"/>
-      <c r="L90" s="2"/>
-      <c r="M90" s="2"/>
+      <c r="K90" s="1"/>
+      <c r="L90" s="1"/>
+      <c r="M90" s="1"/>
       <c r="N90" s="1"/>
+      <c r="O90" s="1"/>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91">
@@ -3929,9 +4813,11 @@
       <c r="H91" s="1"/>
       <c r="I91" s="1"/>
       <c r="J91" s="1"/>
+      <c r="K91" s="1"/>
       <c r="L91" s="1"/>
       <c r="M91" s="1"/>
       <c r="N91" s="1"/>
+      <c r="O91" s="1"/>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92">
@@ -3946,9 +4832,150 @@
       <c r="H92" s="1"/>
       <c r="I92" s="1"/>
       <c r="J92" s="1"/>
+      <c r="K92" s="1"/>
       <c r="L92" s="1"/>
       <c r="M92" s="1"/>
       <c r="N92" s="1"/>
+      <c r="O92" s="1"/>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B96">
+        <v>0</v>
+      </c>
+      <c r="C96">
+        <v>1</v>
+      </c>
+      <c r="D96">
+        <v>2</v>
+      </c>
+      <c r="E96">
+        <v>3</v>
+      </c>
+      <c r="F96">
+        <v>4</v>
+      </c>
+      <c r="G96">
+        <v>5</v>
+      </c>
+      <c r="H96">
+        <v>6</v>
+      </c>
+      <c r="I96">
+        <v>7</v>
+      </c>
+      <c r="J96">
+        <v>8</v>
+      </c>
+      <c r="M96">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>5</v>
+      </c>
+      <c r="B97" s="3"/>
+      <c r="C97" s="3"/>
+      <c r="D97" s="3"/>
+      <c r="E97" s="3"/>
+      <c r="F97" s="3"/>
+      <c r="G97" s="2"/>
+      <c r="H97" s="1"/>
+      <c r="I97" s="1"/>
+      <c r="J97" s="1"/>
+      <c r="L97" s="1"/>
+      <c r="M97" s="1"/>
+      <c r="N97" s="1"/>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>4</v>
+      </c>
+      <c r="B98" s="1"/>
+      <c r="C98" s="1"/>
+      <c r="D98" s="1"/>
+      <c r="E98" s="1"/>
+      <c r="F98" s="2"/>
+      <c r="G98" s="1"/>
+      <c r="H98" s="2"/>
+      <c r="I98" s="1"/>
+      <c r="J98" s="1"/>
+      <c r="L98" s="1"/>
+      <c r="M98" s="1"/>
+      <c r="N98" s="1"/>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>3</v>
+      </c>
+      <c r="B99" s="1"/>
+      <c r="C99" s="1"/>
+      <c r="D99" s="3"/>
+      <c r="E99" s="2"/>
+      <c r="F99" s="1"/>
+      <c r="G99" s="1"/>
+      <c r="H99" s="1"/>
+      <c r="I99" s="2"/>
+      <c r="J99" s="1"/>
+      <c r="L99" s="1"/>
+      <c r="M99" s="3"/>
+      <c r="N99" s="2"/>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>2</v>
+      </c>
+      <c r="B100" s="1"/>
+      <c r="C100" s="1"/>
+      <c r="D100" s="2"/>
+      <c r="E100" s="3"/>
+      <c r="F100" s="3"/>
+      <c r="G100" s="3"/>
+      <c r="H100" s="3"/>
+      <c r="I100" s="3"/>
+      <c r="J100" s="2"/>
+      <c r="L100" s="2"/>
+      <c r="M100" s="2"/>
+      <c r="N100" s="1"/>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>1</v>
+      </c>
+      <c r="B101" s="1"/>
+      <c r="C101" s="2"/>
+      <c r="D101" s="1"/>
+      <c r="E101" s="1"/>
+      <c r="F101" s="1"/>
+      <c r="G101" s="1"/>
+      <c r="H101" s="1"/>
+      <c r="I101" s="1"/>
+      <c r="J101" s="1"/>
+      <c r="L101" s="1"/>
+      <c r="M101" s="1"/>
+      <c r="N101" s="1"/>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>0</v>
+      </c>
+      <c r="B102" s="2"/>
+      <c r="C102" s="1"/>
+      <c r="D102" s="1"/>
+      <c r="E102" s="1"/>
+      <c r="F102" s="1"/>
+      <c r="G102" s="1"/>
+      <c r="H102" s="1"/>
+      <c r="I102" s="1"/>
+      <c r="J102" s="1"/>
+      <c r="L102" s="1"/>
+      <c r="M102" s="1"/>
+      <c r="N102" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>